<commit_message>
add one more mapping
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@79746 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ICEMR/ICEMR protein array/ICEMR submission form v3 ontology mapping.xlsx
+++ b/Load/src/ontology/ICEMR/ICEMR protein array/ICEMR submission form v3 ontology mapping.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="468">
   <si>
     <t>ICEMR_abnormal_bleeding</t>
   </si>
@@ -1417,6 +1417,15 @@
   </si>
   <si>
     <t>Green: categoried consider to remove</t>
+  </si>
+  <si>
+    <t>day of follow up specimen collection from original collection</t>
+  </si>
+  <si>
+    <t>information of informed consent for future use of specimen</t>
+  </si>
+  <si>
+    <t>add to EuPath under ICE/ or use UBERON_0009097 gravid organism (pregnant as display label as ICEMR amazonia project)</t>
   </si>
 </sst>
 </file>
@@ -2583,8 +2592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="C37" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3016,6 +3025,9 @@
       <c r="D20" t="s">
         <v>116</v>
       </c>
+      <c r="F20" t="s">
+        <v>465</v>
+      </c>
       <c r="G20" t="s">
         <v>374</v>
       </c>
@@ -3032,6 +3044,9 @@
       </c>
       <c r="D21" t="s">
         <v>118</v>
+      </c>
+      <c r="F21" t="s">
+        <v>466</v>
       </c>
       <c r="G21" t="s">
         <v>370</v>
@@ -3807,8 +3822,8 @@
       <c r="F59" s="6" t="s">
         <v>443</v>
       </c>
-      <c r="G59" t="s">
-        <v>370</v>
+      <c r="G59" s="4" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -6185,7 +6200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G185"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add term type information to ICEMR protein array terms
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@79762 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ICEMR/ICEMR protein array/ICEMR submission form v3 ontology mapping.xlsx
+++ b/Load/src/ontology/ICEMR/ICEMR protein array/ICEMR submission form v3 ontology mapping.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19100" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="terms.txt" sheetId="1" r:id="rId1"/>
-    <sheet name="relationship" sheetId="2" r:id="rId2"/>
-    <sheet name="ICEMR submission form" sheetId="5" r:id="rId3"/>
+    <sheet name="terms.txt (2)" sheetId="6" r:id="rId1"/>
+    <sheet name="terms.txt" sheetId="1" r:id="rId2"/>
+    <sheet name="relationship" sheetId="2" r:id="rId3"/>
+    <sheet name="ICEMR submission form" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="471">
   <si>
     <t>ICEMR_abnormal_bleeding</t>
   </si>
@@ -1426,13 +1427,22 @@
   </si>
   <si>
     <t>add to EuPath under ICE/ or use UBERON_0009097 gravid organism (pregnant as display label as ICEMR amazonia project)</t>
+  </si>
+  <si>
+    <t>term type</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>variable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1527,6 +1537,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF6600"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -1742,7 +1758,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="194">
+  <cellStyleXfs count="230">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1937,8 +1953,44 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -2066,8 +2118,9 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="194">
+  <cellStyles count="230">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2253,6 +2306,24 @@
     <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2260,6 +2331,24 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="94"/>
   </cellStyles>
@@ -2592,17 +2681,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView topLeftCell="A187" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E84" sqref="E2:F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="35.6640625" customWidth="1"/>
     <col min="2" max="2" width="41" customWidth="1"/>
-    <col min="3" max="3" width="42.33203125" customWidth="1"/>
-    <col min="4" max="4" width="36.5" customWidth="1"/>
-    <col min="5" max="5" width="36.1640625" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" customWidth="1"/>
+    <col min="4" max="4" width="42.33203125" customWidth="1"/>
+    <col min="5" max="5" width="43.5" customWidth="1"/>
     <col min="6" max="6" width="41" customWidth="1"/>
     <col min="7" max="7" width="16.5" customWidth="1"/>
     <col min="8" max="8" width="43.6640625" style="5" customWidth="1"/>
@@ -2670,6 +2759,9 @@
       <c r="D3" t="s">
         <v>80</v>
       </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
       <c r="G3" t="s">
         <v>267</v>
       </c>
@@ -2862,6 +2954,9 @@
       <c r="D12" t="s">
         <v>192</v>
       </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
       <c r="G12" s="2" t="s">
         <v>399</v>
       </c>
@@ -2921,6 +3016,9 @@
       </c>
       <c r="D15" t="s">
         <v>206</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
       </c>
       <c r="G15" t="s">
         <v>401</v>
@@ -3166,6 +3264,9 @@
       <c r="D27" t="s">
         <v>80</v>
       </c>
+      <c r="E27" t="s">
+        <v>202</v>
+      </c>
       <c r="G27" t="s">
         <v>267</v>
       </c>
@@ -4386,6 +4487,2598 @@
       </c>
     </row>
     <row r="96" spans="1:7">
+      <c r="B96" t="s">
+        <v>22</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D96" t="s">
+        <v>20</v>
+      </c>
+      <c r="E96" t="s">
+        <v>270</v>
+      </c>
+      <c r="F96" t="s">
+        <v>269</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7">
+      <c r="B97" t="s">
+        <v>24</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D97" t="s">
+        <v>20</v>
+      </c>
+      <c r="E97" t="s">
+        <v>272</v>
+      </c>
+      <c r="F97" t="s">
+        <v>271</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7">
+      <c r="B98" t="s">
+        <v>26</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D98" t="s">
+        <v>20</v>
+      </c>
+      <c r="E98" t="s">
+        <v>274</v>
+      </c>
+      <c r="F98" t="s">
+        <v>273</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7">
+      <c r="B99" t="s">
+        <v>30</v>
+      </c>
+      <c r="C99" t="s">
+        <v>31</v>
+      </c>
+      <c r="D99" t="s">
+        <v>20</v>
+      </c>
+      <c r="E99" t="s">
+        <v>276</v>
+      </c>
+      <c r="F99" t="s">
+        <v>277</v>
+      </c>
+      <c r="G99" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7">
+      <c r="B100" t="s">
+        <v>50</v>
+      </c>
+      <c r="C100" t="s">
+        <v>51</v>
+      </c>
+      <c r="D100" t="s">
+        <v>20</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7">
+      <c r="B101" t="s">
+        <v>98</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D101" t="s">
+        <v>20</v>
+      </c>
+      <c r="E101" t="s">
+        <v>2</v>
+      </c>
+      <c r="F101" t="s">
+        <v>3</v>
+      </c>
+      <c r="G101" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7">
+      <c r="B102" t="s">
+        <v>104</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D102" t="s">
+        <v>20</v>
+      </c>
+      <c r="E102" t="s">
+        <v>202</v>
+      </c>
+      <c r="F102" t="s">
+        <v>203</v>
+      </c>
+      <c r="G102" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7">
+      <c r="B103" t="s">
+        <v>114</v>
+      </c>
+      <c r="C103" t="s">
+        <v>115</v>
+      </c>
+      <c r="D103" t="s">
+        <v>20</v>
+      </c>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+    </row>
+    <row r="104" spans="2:7">
+      <c r="B104" t="s">
+        <v>160</v>
+      </c>
+      <c r="C104" t="s">
+        <v>161</v>
+      </c>
+      <c r="D104" t="s">
+        <v>20</v>
+      </c>
+      <c r="E104" s="5"/>
+      <c r="F104" s="5"/>
+    </row>
+    <row r="105" spans="2:7">
+      <c r="B105" t="s">
+        <v>208</v>
+      </c>
+      <c r="C105" t="s">
+        <v>209</v>
+      </c>
+      <c r="D105" t="s">
+        <v>20</v>
+      </c>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+    </row>
+    <row r="106" spans="2:7">
+      <c r="B106" t="s">
+        <v>212</v>
+      </c>
+      <c r="C106" t="s">
+        <v>213</v>
+      </c>
+      <c r="D106" t="s">
+        <v>20</v>
+      </c>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+    </row>
+    <row r="107" spans="2:7">
+      <c r="B107" t="s">
+        <v>232</v>
+      </c>
+      <c r="C107" t="s">
+        <v>233</v>
+      </c>
+      <c r="D107" t="s">
+        <v>20</v>
+      </c>
+      <c r="E107" t="s">
+        <v>285</v>
+      </c>
+      <c r="F107" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7">
+      <c r="B108" t="s">
+        <v>238</v>
+      </c>
+      <c r="C108" t="s">
+        <v>239</v>
+      </c>
+      <c r="D108" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7">
+      <c r="B109" t="s">
+        <v>110</v>
+      </c>
+      <c r="C109" t="s">
+        <v>111</v>
+      </c>
+      <c r="D109" t="s">
+        <v>40</v>
+      </c>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+    </row>
+    <row r="110" spans="2:7">
+      <c r="B110" t="s">
+        <v>6</v>
+      </c>
+      <c r="C110" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110" t="s">
+        <v>50</v>
+      </c>
+      <c r="E110" t="s">
+        <v>246</v>
+      </c>
+      <c r="F110" t="s">
+        <v>244</v>
+      </c>
+      <c r="G110" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7">
+      <c r="B111" t="s">
+        <v>120</v>
+      </c>
+      <c r="C111" t="s">
+        <v>121</v>
+      </c>
+      <c r="D111" t="s">
+        <v>50</v>
+      </c>
+      <c r="E111" s="5"/>
+      <c r="F111" s="5"/>
+    </row>
+    <row r="112" spans="2:7">
+      <c r="B112" t="s">
+        <v>134</v>
+      </c>
+      <c r="C112" t="s">
+        <v>135</v>
+      </c>
+      <c r="D112" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7">
+      <c r="B113" t="s">
+        <v>138</v>
+      </c>
+      <c r="C113" t="s">
+        <v>139</v>
+      </c>
+      <c r="D113" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7">
+      <c r="B114" t="s">
+        <v>228</v>
+      </c>
+      <c r="C114" t="s">
+        <v>229</v>
+      </c>
+      <c r="D114" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7">
+      <c r="B115" t="s">
+        <v>16</v>
+      </c>
+      <c r="C115" t="s">
+        <v>17</v>
+      </c>
+      <c r="D115" t="s">
+        <v>62</v>
+      </c>
+      <c r="E115" t="s">
+        <v>264</v>
+      </c>
+      <c r="F115" t="s">
+        <v>263</v>
+      </c>
+      <c r="G115" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7">
+      <c r="B116" t="s">
+        <v>112</v>
+      </c>
+      <c r="C116" t="s">
+        <v>113</v>
+      </c>
+      <c r="D116" t="s">
+        <v>110</v>
+      </c>
+      <c r="E116" s="5"/>
+      <c r="F116" s="5"/>
+    </row>
+    <row r="117" spans="2:7">
+      <c r="B117" t="s">
+        <v>14</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D117" t="s">
+        <v>130</v>
+      </c>
+      <c r="E117" t="s">
+        <v>261</v>
+      </c>
+      <c r="F117" t="s">
+        <v>260</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7">
+      <c r="B118" t="s">
+        <v>226</v>
+      </c>
+      <c r="C118" t="s">
+        <v>227</v>
+      </c>
+      <c r="D118" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7">
+      <c r="B119" t="s">
+        <v>230</v>
+      </c>
+      <c r="C119" t="s">
+        <v>231</v>
+      </c>
+      <c r="D119" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7">
+      <c r="B120" t="s">
+        <v>224</v>
+      </c>
+      <c r="C120" s="56" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7">
+      <c r="B121" t="s">
+        <v>82</v>
+      </c>
+      <c r="C121" t="s">
+        <v>83</v>
+      </c>
+      <c r="D121" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7">
+      <c r="B122" t="s">
+        <v>54</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D122" t="s">
+        <v>206</v>
+      </c>
+      <c r="E122" s="5"/>
+      <c r="F122" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="G122" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7">
+      <c r="B123" t="s">
+        <v>122</v>
+      </c>
+      <c r="C123" t="s">
+        <v>123</v>
+      </c>
+      <c r="D123" t="s">
+        <v>224</v>
+      </c>
+      <c r="E123" s="5"/>
+      <c r="F123" s="5"/>
+    </row>
+    <row r="124" spans="2:7">
+      <c r="B124" t="s">
+        <v>12</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E124" t="s">
+        <v>252</v>
+      </c>
+      <c r="F124" t="s">
+        <v>251</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7">
+      <c r="B125" t="s">
+        <v>20</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7">
+      <c r="B126" t="s">
+        <v>40</v>
+      </c>
+      <c r="C126" t="s">
+        <v>41</v>
+      </c>
+      <c r="E126" t="s">
+        <v>360</v>
+      </c>
+      <c r="F126" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G126" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7">
+      <c r="B127" t="s">
+        <v>56</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E127" s="5"/>
+      <c r="F127" t="s">
+        <v>365</v>
+      </c>
+      <c r="G127" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7">
+      <c r="B128" t="s">
+        <v>102</v>
+      </c>
+      <c r="C128" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6">
+      <c r="B129" t="s">
+        <v>140</v>
+      </c>
+      <c r="C129" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6">
+      <c r="B130" t="s">
+        <v>198</v>
+      </c>
+      <c r="C130" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="131" spans="2:6">
+      <c r="B131" t="s">
+        <v>210</v>
+      </c>
+      <c r="C131" t="s">
+        <v>211</v>
+      </c>
+      <c r="E131" s="5"/>
+      <c r="F131" s="5"/>
+    </row>
+    <row r="134" spans="2:6">
+      <c r="B134" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="136" spans="2:6">
+      <c r="B136" t="s">
+        <v>397</v>
+      </c>
+      <c r="C136" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="D136" s="55"/>
+    </row>
+    <row r="137" spans="2:6">
+      <c r="C137" s="55" t="s">
+        <v>298</v>
+      </c>
+      <c r="D137" s="55"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I137"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="41" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="43.6640625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="57" customFormat="1">
+      <c r="A1" s="57" t="s">
+        <v>396</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>259</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>398</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>255</v>
+      </c>
+      <c r="F1" s="57" t="s">
+        <v>256</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>257</v>
+      </c>
+      <c r="H1" s="83" t="s">
+        <v>468</v>
+      </c>
+      <c r="I1" s="58"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G2" t="s">
+        <v>356</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" t="s">
+        <v>267</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" t="s">
+        <v>242</v>
+      </c>
+      <c r="F4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G4" t="s">
+        <v>356</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>370</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" t="s">
+        <v>266</v>
+      </c>
+      <c r="F6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>280</v>
+      </c>
+      <c r="F7" t="s">
+        <v>279</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18" customHeight="1">
+      <c r="A8" t="s">
+        <v>310</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" t="s">
+        <v>402</v>
+      </c>
+      <c r="G8" t="s">
+        <v>369</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
+        <v>356</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>297</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>192</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>391</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="G13" t="s">
+        <v>370</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>291</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="G14" t="s">
+        <v>400</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>296</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>206</v>
+      </c>
+      <c r="G15" t="s">
+        <v>401</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>330</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s">
+        <v>146</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" t="s">
+        <v>330</v>
+      </c>
+      <c r="G16" t="s">
+        <v>366</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" t="s">
+        <v>418</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="56" t="s">
+        <v>384</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="F18" t="s">
+        <v>372</v>
+      </c>
+      <c r="G18" t="s">
+        <v>431</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>385</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="G19" t="s">
+        <v>373</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>311</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>116</v>
+      </c>
+      <c r="F20" t="s">
+        <v>465</v>
+      </c>
+      <c r="G20" t="s">
+        <v>374</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>392</v>
+      </c>
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21" t="s">
+        <v>466</v>
+      </c>
+      <c r="G21" t="s">
+        <v>370</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>340</v>
+      </c>
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" t="s">
+        <v>377</v>
+      </c>
+      <c r="G22" t="s">
+        <v>379</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>341</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" t="s">
+        <v>378</v>
+      </c>
+      <c r="G23" t="s">
+        <v>379</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" t="s">
+        <v>130</v>
+      </c>
+      <c r="F24" t="s">
+        <v>406</v>
+      </c>
+      <c r="G24" s="60" t="s">
+        <v>426</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" t="s">
+        <v>405</v>
+      </c>
+      <c r="G25" t="s">
+        <v>422</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>342</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" t="s">
+        <v>404</v>
+      </c>
+      <c r="G26" t="s">
+        <v>403</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="56" t="s">
+        <v>295</v>
+      </c>
+      <c r="B27" t="s">
+        <v>202</v>
+      </c>
+      <c r="C27" t="s">
+        <v>203</v>
+      </c>
+      <c r="D27" t="s">
+        <v>80</v>
+      </c>
+      <c r="G27" t="s">
+        <v>267</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" t="s">
+        <v>407</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" t="s">
+        <v>287</v>
+      </c>
+      <c r="F29" t="s">
+        <v>349</v>
+      </c>
+      <c r="G29" t="s">
+        <v>267</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>302</v>
+      </c>
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" t="s">
+        <v>192</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="G30" t="s">
+        <v>267</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>305</v>
+      </c>
+      <c r="B31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" t="s">
+        <v>192</v>
+      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="G31" t="s">
+        <v>370</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>299</v>
+      </c>
+      <c r="B32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" t="s">
+        <v>192</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="G32" t="s">
+        <v>267</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>382</v>
+      </c>
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" t="s">
+        <v>192</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" t="s">
+        <v>409</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>312</v>
+      </c>
+      <c r="B34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" t="s">
+        <v>150</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="G34" t="s">
+        <v>267</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>344</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" t="s">
+        <v>130</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="G35" t="s">
+        <v>267</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>383</v>
+      </c>
+      <c r="B36" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" t="s">
+        <v>150</v>
+      </c>
+      <c r="E36" t="s">
+        <v>375</v>
+      </c>
+      <c r="F36" t="s">
+        <v>376</v>
+      </c>
+      <c r="G36" t="s">
+        <v>267</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>387</v>
+      </c>
+      <c r="B37" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="G37" t="s">
+        <v>370</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" t="s">
+        <v>146</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G38" t="s">
+        <v>267</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>389</v>
+      </c>
+      <c r="B39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="G39" t="s">
+        <v>370</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="56" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" t="s">
+        <v>206</v>
+      </c>
+      <c r="G40" t="s">
+        <v>437</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="G41" t="s">
+        <v>356</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>381</v>
+      </c>
+      <c r="B42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" t="s">
+        <v>125</v>
+      </c>
+      <c r="D42" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="G42" t="s">
+        <v>417</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>127</v>
+      </c>
+      <c r="B43" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" t="s">
+        <v>146</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G43" t="s">
+        <v>267</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>129</v>
+      </c>
+      <c r="B44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" t="s">
+        <v>176</v>
+      </c>
+      <c r="E44" s="5"/>
+      <c r="F44" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" t="s">
+        <v>130</v>
+      </c>
+      <c r="C45" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="G45" t="s">
+        <v>421</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C46" t="s">
+        <v>133</v>
+      </c>
+      <c r="D46" t="s">
+        <v>176</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>333</v>
+      </c>
+      <c r="B47" t="s">
+        <v>136</v>
+      </c>
+      <c r="C47" t="s">
+        <v>137</v>
+      </c>
+      <c r="D47" t="s">
+        <v>156</v>
+      </c>
+      <c r="G47" s="60" t="s">
+        <v>439</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="56" t="s">
+        <v>343</v>
+      </c>
+      <c r="B48" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" t="s">
+        <v>143</v>
+      </c>
+      <c r="D48" t="s">
+        <v>72</v>
+      </c>
+      <c r="G48" s="60" t="s">
+        <v>425</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>390</v>
+      </c>
+      <c r="B49" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" t="s">
+        <v>145</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" t="s">
+        <v>427</v>
+      </c>
+      <c r="G49" t="s">
+        <v>370</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
+        <v>147</v>
+      </c>
+      <c r="B50" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" t="s">
+        <v>428</v>
+      </c>
+      <c r="F50" t="s">
+        <v>429</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>149</v>
+      </c>
+      <c r="B51" t="s">
+        <v>148</v>
+      </c>
+      <c r="C51" t="s">
+        <v>149</v>
+      </c>
+      <c r="D51" t="s">
+        <v>176</v>
+      </c>
+      <c r="F51" t="s">
+        <v>430</v>
+      </c>
+      <c r="G51" t="s">
+        <v>418</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>151</v>
+      </c>
+      <c r="B52" t="s">
+        <v>150</v>
+      </c>
+      <c r="C52" s="59" t="s">
+        <v>151</v>
+      </c>
+      <c r="D52" t="s">
+        <v>28</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>334</v>
+      </c>
+      <c r="B53" t="s">
+        <v>152</v>
+      </c>
+      <c r="C53" t="s">
+        <v>153</v>
+      </c>
+      <c r="D53" t="s">
+        <v>156</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>338</v>
+      </c>
+      <c r="B54" t="s">
+        <v>154</v>
+      </c>
+      <c r="C54" t="s">
+        <v>155</v>
+      </c>
+      <c r="D54" t="s">
+        <v>156</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>157</v>
+      </c>
+      <c r="B55" t="s">
+        <v>156</v>
+      </c>
+      <c r="C55" s="56" t="s">
+        <v>157</v>
+      </c>
+      <c r="D55" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" t="s">
+        <v>388</v>
+      </c>
+      <c r="B56" t="s">
+        <v>158</v>
+      </c>
+      <c r="C56" s="63" t="s">
+        <v>159</v>
+      </c>
+      <c r="D56" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="5"/>
+      <c r="F56" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="G56" t="s">
+        <v>370</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>339</v>
+      </c>
+      <c r="B57" t="s">
+        <v>162</v>
+      </c>
+      <c r="C57" s="63" t="s">
+        <v>163</v>
+      </c>
+      <c r="D57" t="s">
+        <v>156</v>
+      </c>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" t="s">
+        <v>441</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>337</v>
+      </c>
+      <c r="B58" t="s">
+        <v>164</v>
+      </c>
+      <c r="C58" s="63" t="s">
+        <v>165</v>
+      </c>
+      <c r="D58" t="s">
+        <v>156</v>
+      </c>
+      <c r="E58" s="5"/>
+      <c r="F58" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="G58" t="s">
+        <v>370</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>315</v>
+      </c>
+      <c r="B59" t="s">
+        <v>174</v>
+      </c>
+      <c r="C59" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="D59" t="s">
+        <v>150</v>
+      </c>
+      <c r="E59" s="5"/>
+      <c r="F59" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
+        <v>386</v>
+      </c>
+      <c r="B60" t="s">
+        <v>176</v>
+      </c>
+      <c r="C60" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="D60" t="s">
+        <v>130</v>
+      </c>
+      <c r="E60" s="5"/>
+      <c r="F60" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="G60" t="s">
+        <v>418</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" t="s">
+        <v>331</v>
+      </c>
+      <c r="B61" t="s">
+        <v>186</v>
+      </c>
+      <c r="C61" s="63" t="s">
+        <v>187</v>
+      </c>
+      <c r="D61" t="s">
+        <v>156</v>
+      </c>
+      <c r="E61" s="5"/>
+      <c r="F61" s="64" t="s">
+        <v>444</v>
+      </c>
+      <c r="G61" s="60" t="s">
+        <v>445</v>
+      </c>
+      <c r="H61" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" t="s">
+        <v>325</v>
+      </c>
+      <c r="B62" t="s">
+        <v>188</v>
+      </c>
+      <c r="C62" t="s">
+        <v>189</v>
+      </c>
+      <c r="D62" t="s">
+        <v>146</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="F62" s="61" t="s">
+        <v>327</v>
+      </c>
+      <c r="G62" t="s">
+        <v>356</v>
+      </c>
+      <c r="H62" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" t="s">
+        <v>319</v>
+      </c>
+      <c r="B63" t="s">
+        <v>190</v>
+      </c>
+      <c r="C63" t="s">
+        <v>191</v>
+      </c>
+      <c r="D63" t="s">
+        <v>146</v>
+      </c>
+      <c r="E63" s="62" t="s">
+        <v>353</v>
+      </c>
+      <c r="F63" s="62" t="s">
+        <v>352</v>
+      </c>
+      <c r="G63" t="s">
+        <v>400</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" t="s">
+        <v>193</v>
+      </c>
+      <c r="B64" t="s">
+        <v>192</v>
+      </c>
+      <c r="C64" s="63" t="s">
+        <v>193</v>
+      </c>
+      <c r="D64" t="s">
+        <v>206</v>
+      </c>
+      <c r="F64" s="62" t="s">
+        <v>447</v>
+      </c>
+      <c r="G64" t="s">
+        <v>446</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>380</v>
+      </c>
+      <c r="B65" t="s">
+        <v>196</v>
+      </c>
+      <c r="C65" s="63" t="s">
+        <v>197</v>
+      </c>
+      <c r="D65" t="s">
+        <v>80</v>
+      </c>
+      <c r="F65" s="62" t="s">
+        <v>448</v>
+      </c>
+      <c r="G65" t="s">
+        <v>449</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>318</v>
+      </c>
+      <c r="B66" t="s">
+        <v>200</v>
+      </c>
+      <c r="C66" t="s">
+        <v>201</v>
+      </c>
+      <c r="D66" t="s">
+        <v>146</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="G66" t="s">
+        <v>400</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>205</v>
+      </c>
+      <c r="B67" t="s">
+        <v>204</v>
+      </c>
+      <c r="C67" t="s">
+        <v>205</v>
+      </c>
+      <c r="D67" t="s">
+        <v>146</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="G67" t="s">
+        <v>356</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>207</v>
+      </c>
+      <c r="B68" t="s">
+        <v>206</v>
+      </c>
+      <c r="C68" s="56" t="s">
+        <v>207</v>
+      </c>
+      <c r="D68" t="s">
+        <v>78</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="G68" t="s">
+        <v>413</v>
+      </c>
+      <c r="H68" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>309</v>
+      </c>
+      <c r="B69" t="s">
+        <v>214</v>
+      </c>
+      <c r="C69" t="s">
+        <v>215</v>
+      </c>
+      <c r="D69" t="s">
+        <v>116</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="G69" t="s">
+        <v>435</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>288</v>
+      </c>
+      <c r="B70" t="s">
+        <v>218</v>
+      </c>
+      <c r="C70" t="s">
+        <v>219</v>
+      </c>
+      <c r="D70" t="s">
+        <v>80</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="H70" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>306</v>
+      </c>
+      <c r="B71" t="s">
+        <v>216</v>
+      </c>
+      <c r="C71" t="s">
+        <v>217</v>
+      </c>
+      <c r="D71" t="s">
+        <v>116</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="H71" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" t="s">
+        <v>316</v>
+      </c>
+      <c r="B72" t="s">
+        <v>222</v>
+      </c>
+      <c r="C72" t="s">
+        <v>223</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="G72" t="s">
+        <v>436</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>317</v>
+      </c>
+      <c r="B73" t="s">
+        <v>220</v>
+      </c>
+      <c r="C73" t="s">
+        <v>221</v>
+      </c>
+      <c r="D73" t="s">
+        <v>62</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" s="56" customFormat="1">
+      <c r="A74" s="56" t="s">
+        <v>332</v>
+      </c>
+      <c r="B74" s="56" t="s">
+        <v>234</v>
+      </c>
+      <c r="C74" s="63" t="s">
+        <v>235</v>
+      </c>
+      <c r="D74" s="56" t="s">
+        <v>156</v>
+      </c>
+      <c r="F74" s="66" t="s">
+        <v>450</v>
+      </c>
+      <c r="G74" s="56" t="s">
+        <v>403</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="I74" s="65"/>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" t="s">
+        <v>237</v>
+      </c>
+      <c r="B75" t="s">
+        <v>236</v>
+      </c>
+      <c r="C75" s="63" t="s">
+        <v>237</v>
+      </c>
+      <c r="D75" t="s">
+        <v>176</v>
+      </c>
+      <c r="F75" s="66" t="s">
+        <v>451</v>
+      </c>
+      <c r="G75" s="67" t="s">
+        <v>286</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" t="s">
+        <v>393</v>
+      </c>
+      <c r="B76" t="s">
+        <v>166</v>
+      </c>
+      <c r="C76" s="63" t="s">
+        <v>167</v>
+      </c>
+      <c r="D76" t="s">
+        <v>72</v>
+      </c>
+      <c r="F76" s="56" t="s">
+        <v>452</v>
+      </c>
+      <c r="G76" s="56" t="s">
+        <v>453</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" t="s">
+        <v>393</v>
+      </c>
+      <c r="B77" t="s">
+        <v>172</v>
+      </c>
+      <c r="C77" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="D77" t="s">
+        <v>72</v>
+      </c>
+      <c r="F77" s="56" t="s">
+        <v>454</v>
+      </c>
+      <c r="G77" s="67" t="s">
+        <v>394</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" t="s">
+        <v>393</v>
+      </c>
+      <c r="B78" t="s">
+        <v>178</v>
+      </c>
+      <c r="C78" s="63" t="s">
+        <v>179</v>
+      </c>
+      <c r="D78" t="s">
+        <v>72</v>
+      </c>
+      <c r="F78" s="56" t="s">
+        <v>455</v>
+      </c>
+      <c r="H78" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" t="s">
+        <v>393</v>
+      </c>
+      <c r="B79" t="s">
+        <v>180</v>
+      </c>
+      <c r="C79" s="63" t="s">
+        <v>181</v>
+      </c>
+      <c r="D79" t="s">
+        <v>72</v>
+      </c>
+      <c r="F79" s="56" t="s">
+        <v>458</v>
+      </c>
+      <c r="G79" t="s">
+        <v>395</v>
+      </c>
+      <c r="H79" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" t="s">
+        <v>393</v>
+      </c>
+      <c r="B80" t="s">
+        <v>168</v>
+      </c>
+      <c r="C80" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="D80" t="s">
+        <v>156</v>
+      </c>
+      <c r="F80" s="56" t="s">
+        <v>456</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" t="s">
+        <v>393</v>
+      </c>
+      <c r="B81" t="s">
+        <v>170</v>
+      </c>
+      <c r="C81" s="63" t="s">
+        <v>171</v>
+      </c>
+      <c r="D81" t="s">
+        <v>156</v>
+      </c>
+      <c r="F81" s="56" t="s">
+        <v>459</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" t="s">
+        <v>393</v>
+      </c>
+      <c r="B82" t="s">
+        <v>182</v>
+      </c>
+      <c r="C82" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="D82" t="s">
+        <v>156</v>
+      </c>
+      <c r="F82" s="56" t="s">
+        <v>457</v>
+      </c>
+      <c r="H82" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" t="s">
+        <v>393</v>
+      </c>
+      <c r="B83" t="s">
+        <v>184</v>
+      </c>
+      <c r="C83" s="63" t="s">
+        <v>185</v>
+      </c>
+      <c r="D83" t="s">
+        <v>156</v>
+      </c>
+      <c r="F83" s="56" t="s">
+        <v>460</v>
+      </c>
+      <c r="H83" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" t="s">
+        <v>393</v>
+      </c>
+      <c r="B84" t="s">
+        <v>194</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D84" t="s">
+        <v>206</v>
+      </c>
+      <c r="E84" t="s">
+        <v>249</v>
+      </c>
+      <c r="F84" t="s">
+        <v>248</v>
+      </c>
+      <c r="G84" t="s">
+        <v>282</v>
+      </c>
+      <c r="H84" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="C85" s="6"/>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="C86" s="79" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="C87" s="80" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="C88" s="81" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="C89" s="82" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="C90" s="6"/>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="C91" s="6"/>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="C92" s="6"/>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="C93" s="6"/>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="C94" s="6"/>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="B95" t="s">
+        <v>10</v>
+      </c>
+      <c r="C95" t="s">
+        <v>11</v>
+      </c>
+      <c r="D95" t="s">
+        <v>20</v>
+      </c>
+      <c r="E95" t="s">
+        <v>249</v>
+      </c>
+      <c r="F95" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
       <c r="B96" t="s">
         <v>22</v>
       </c>
@@ -4935,7 +7628,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C112"/>
   <sheetViews>
@@ -6196,12 +8889,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G185"/>
+  <dimension ref="A1:G206"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6929,458 +9622,914 @@
         <v>319</v>
       </c>
     </row>
-    <row r="65" spans="7:7">
+    <row r="65" spans="3:7">
       <c r="G65" s="76" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="66" spans="7:7">
+    <row r="66" spans="3:7">
       <c r="G66" s="76" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="67" spans="7:7">
+    <row r="67" spans="3:7">
       <c r="G67" s="74" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="68" spans="7:7">
+    <row r="68" spans="3:7">
       <c r="G68" s="74" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="69" spans="7:7">
+    <row r="69" spans="3:7">
       <c r="G69" s="75" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="70" spans="7:7">
+    <row r="70" spans="3:7">
       <c r="G70" s="74" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="71" spans="7:7">
+    <row r="71" spans="3:7">
       <c r="G71" s="74" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="72" spans="7:7">
+    <row r="72" spans="3:7">
       <c r="G72" s="74" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="73" spans="7:7">
+    <row r="73" spans="3:7">
       <c r="G73" s="74" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="74" spans="7:7">
+    <row r="74" spans="3:7">
+      <c r="C74"/>
+      <c r="D74"/>
       <c r="G74" s="74" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="75" spans="7:7">
+    <row r="75" spans="3:7">
+      <c r="C75"/>
+      <c r="D75"/>
       <c r="G75" s="75" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="76" spans="7:7">
+    <row r="76" spans="3:7">
+      <c r="C76"/>
+      <c r="D76"/>
       <c r="G76" s="76" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="77" spans="7:7">
-      <c r="G77" s="75"/>
-    </row>
-    <row r="78" spans="7:7">
-      <c r="G78" s="75"/>
-    </row>
-    <row r="79" spans="7:7">
-      <c r="G79" s="75"/>
-    </row>
-    <row r="80" spans="7:7">
-      <c r="G80" s="75"/>
-    </row>
-    <row r="81" spans="7:7">
-      <c r="G81" s="75"/>
-    </row>
-    <row r="82" spans="7:7">
-      <c r="G82" s="75"/>
-    </row>
-    <row r="83" spans="7:7">
-      <c r="G83" s="75"/>
-    </row>
-    <row r="84" spans="7:7">
-      <c r="G84" s="75"/>
-    </row>
-    <row r="85" spans="7:7">
-      <c r="G85" s="75"/>
-    </row>
-    <row r="86" spans="7:7">
-      <c r="G86" s="75"/>
-    </row>
-    <row r="87" spans="7:7">
-      <c r="G87" s="75"/>
-    </row>
-    <row r="88" spans="7:7">
-      <c r="G88" s="75"/>
-    </row>
-    <row r="89" spans="7:7">
-      <c r="G89" s="75"/>
-    </row>
-    <row r="90" spans="7:7">
-      <c r="G90" s="75"/>
-    </row>
-    <row r="91" spans="7:7">
-      <c r="G91" s="75"/>
-    </row>
-    <row r="92" spans="7:7">
-      <c r="G92" s="75"/>
-    </row>
-    <row r="93" spans="7:7">
-      <c r="G93" s="75"/>
-    </row>
-    <row r="94" spans="7:7">
-      <c r="G94" s="75"/>
-    </row>
-    <row r="95" spans="7:7">
-      <c r="G95" s="75"/>
-    </row>
-    <row r="96" spans="7:7">
-      <c r="G96" s="75"/>
-    </row>
-    <row r="97" spans="7:7">
-      <c r="G97" s="75"/>
-    </row>
-    <row r="98" spans="7:7">
-      <c r="G98" s="75"/>
-    </row>
-    <row r="99" spans="7:7">
-      <c r="G99" s="75"/>
-    </row>
-    <row r="100" spans="7:7">
-      <c r="G100" s="75"/>
-    </row>
-    <row r="101" spans="7:7">
-      <c r="G101" s="75"/>
-    </row>
-    <row r="102" spans="7:7">
-      <c r="G102" s="75"/>
-    </row>
-    <row r="103" spans="7:7">
-      <c r="G103" s="75"/>
-    </row>
-    <row r="104" spans="7:7">
-      <c r="G104" s="75"/>
-    </row>
-    <row r="105" spans="7:7">
-      <c r="G105" s="75"/>
-    </row>
-    <row r="106" spans="7:7">
-      <c r="G106" s="75"/>
-    </row>
-    <row r="107" spans="7:7">
-      <c r="G107" s="75"/>
-    </row>
-    <row r="108" spans="7:7">
-      <c r="G108" s="75"/>
-    </row>
-    <row r="109" spans="7:7">
-      <c r="G109" s="75"/>
-    </row>
-    <row r="110" spans="7:7">
-      <c r="G110" s="75"/>
-    </row>
-    <row r="111" spans="7:7">
-      <c r="G111" s="75"/>
-    </row>
-    <row r="112" spans="7:7">
-      <c r="G112" s="75"/>
-    </row>
-    <row r="113" spans="7:7">
-      <c r="G113" s="75"/>
-    </row>
-    <row r="114" spans="7:7">
-      <c r="G114" s="75"/>
-    </row>
-    <row r="115" spans="7:7">
-      <c r="G115" s="75"/>
-    </row>
-    <row r="116" spans="7:7">
-      <c r="G116" s="75"/>
-    </row>
-    <row r="117" spans="7:7">
-      <c r="G117" s="75"/>
-    </row>
-    <row r="118" spans="7:7">
-      <c r="G118" s="75"/>
-    </row>
-    <row r="119" spans="7:7">
-      <c r="G119" s="75"/>
-    </row>
-    <row r="120" spans="7:7">
-      <c r="G120" s="75"/>
-    </row>
-    <row r="121" spans="7:7">
-      <c r="G121" s="75"/>
-    </row>
-    <row r="122" spans="7:7">
-      <c r="G122" s="75"/>
-    </row>
-    <row r="123" spans="7:7">
-      <c r="G123" s="75"/>
-    </row>
-    <row r="124" spans="7:7">
-      <c r="G124" s="75"/>
-    </row>
-    <row r="125" spans="7:7">
-      <c r="G125" s="75"/>
-    </row>
-    <row r="126" spans="7:7">
-      <c r="G126" s="75"/>
-    </row>
-    <row r="127" spans="7:7">
-      <c r="G127" s="75"/>
-    </row>
-    <row r="128" spans="7:7">
-      <c r="G128" s="75"/>
-    </row>
-    <row r="129" spans="7:7">
-      <c r="G129" s="75"/>
-    </row>
-    <row r="130" spans="7:7">
-      <c r="G130" s="75"/>
-    </row>
-    <row r="131" spans="7:7">
-      <c r="G131" s="75"/>
-    </row>
-    <row r="132" spans="7:7">
-      <c r="G132" s="75"/>
-    </row>
-    <row r="133" spans="7:7">
-      <c r="G133" s="75"/>
-    </row>
-    <row r="134" spans="7:7">
-      <c r="G134" s="75"/>
-    </row>
-    <row r="135" spans="7:7">
-      <c r="G135" s="75"/>
-    </row>
-    <row r="136" spans="7:7">
-      <c r="G136" s="75"/>
-    </row>
-    <row r="137" spans="7:7">
-      <c r="G137" s="75"/>
-    </row>
-    <row r="138" spans="7:7">
-      <c r="G138" s="75"/>
-    </row>
-    <row r="139" spans="7:7">
-      <c r="G139" s="75"/>
-    </row>
-    <row r="140" spans="7:7">
-      <c r="G140" s="75"/>
-    </row>
-    <row r="141" spans="7:7">
-      <c r="G141" s="75"/>
-    </row>
-    <row r="142" spans="7:7">
-      <c r="G142" s="75"/>
-    </row>
-    <row r="143" spans="7:7">
-      <c r="G143" s="75"/>
-    </row>
-    <row r="144" spans="7:7">
-      <c r="G144" s="75"/>
-    </row>
-    <row r="145" spans="7:7">
-      <c r="G145" s="75"/>
-    </row>
-    <row r="146" spans="7:7">
-      <c r="G146" s="75"/>
-    </row>
-    <row r="147" spans="7:7">
-      <c r="G147" s="75"/>
-    </row>
-    <row r="148" spans="7:7">
-      <c r="G148" s="75"/>
-    </row>
-    <row r="149" spans="7:7">
-      <c r="G149" s="75"/>
-    </row>
-    <row r="150" spans="7:7">
-      <c r="G150" s="75"/>
-    </row>
-    <row r="151" spans="7:7">
-      <c r="G151" s="75"/>
-    </row>
-    <row r="152" spans="7:7">
-      <c r="G152" s="75"/>
-    </row>
-    <row r="153" spans="7:7">
-      <c r="G153" s="75"/>
-    </row>
-    <row r="154" spans="7:7">
-      <c r="G154" s="75"/>
-    </row>
-    <row r="155" spans="7:7">
-      <c r="G155" s="75"/>
-    </row>
-    <row r="156" spans="7:7">
-      <c r="G156" s="75"/>
-    </row>
-    <row r="157" spans="7:7">
-      <c r="G157" s="75"/>
-    </row>
-    <row r="158" spans="7:7">
-      <c r="G158" s="75"/>
-    </row>
-    <row r="159" spans="7:7">
-      <c r="G159" s="75"/>
-    </row>
-    <row r="160" spans="7:7">
-      <c r="G160" s="75"/>
-    </row>
-    <row r="161" spans="7:7">
-      <c r="G161" s="75"/>
-    </row>
-    <row r="162" spans="7:7">
-      <c r="G162" s="75"/>
-    </row>
-    <row r="163" spans="7:7">
-      <c r="G163" s="75"/>
-    </row>
-    <row r="164" spans="7:7">
-      <c r="G164" s="75"/>
-    </row>
-    <row r="165" spans="7:7">
-      <c r="G165" s="75"/>
-    </row>
-    <row r="166" spans="7:7">
-      <c r="G166" s="75"/>
-    </row>
-    <row r="167" spans="7:7">
-      <c r="G167" s="75"/>
-    </row>
-    <row r="168" spans="7:7">
-      <c r="G168" s="75"/>
-    </row>
-    <row r="169" spans="7:7">
-      <c r="G169" s="75"/>
-    </row>
-    <row r="170" spans="7:7">
-      <c r="G170" s="75"/>
-    </row>
-    <row r="171" spans="7:7">
-      <c r="G171" s="75"/>
-    </row>
-    <row r="172" spans="7:7">
-      <c r="G172" s="75"/>
-    </row>
-    <row r="173" spans="7:7">
-      <c r="G173" s="75"/>
-    </row>
-    <row r="174" spans="7:7">
-      <c r="G174" s="75"/>
-    </row>
-    <row r="175" spans="7:7">
-      <c r="G175" s="75"/>
-    </row>
-    <row r="176" spans="7:7">
-      <c r="G176" s="75"/>
-    </row>
-    <row r="177" spans="7:7">
-      <c r="G177" s="75"/>
-    </row>
-    <row r="178" spans="7:7">
-      <c r="G178" s="76"/>
-    </row>
-    <row r="179" spans="7:7">
-      <c r="G179" s="76"/>
-    </row>
-    <row r="180" spans="7:7">
-      <c r="G180" s="76"/>
-    </row>
-    <row r="181" spans="7:7">
-      <c r="G181" s="76"/>
-    </row>
-    <row r="182" spans="7:7">
-      <c r="G182" s="76"/>
-    </row>
-    <row r="183" spans="7:7">
-      <c r="G183" s="74"/>
-    </row>
-    <row r="184" spans="7:7">
-      <c r="G184" s="74"/>
-    </row>
-    <row r="185" spans="7:7">
-      <c r="G185" s="74"/>
+    <row r="77" spans="3:7">
+      <c r="C77"/>
+      <c r="D77"/>
+      <c r="E77" s="75"/>
+      <c r="G77"/>
+    </row>
+    <row r="78" spans="3:7">
+      <c r="C78"/>
+      <c r="D78"/>
+      <c r="E78" s="75"/>
+      <c r="G78"/>
+    </row>
+    <row r="79" spans="3:7">
+      <c r="C79"/>
+      <c r="D79"/>
+      <c r="E79" s="75"/>
+      <c r="G79"/>
+    </row>
+    <row r="80" spans="3:7">
+      <c r="C80"/>
+      <c r="D80"/>
+      <c r="E80" s="75"/>
+      <c r="G80"/>
+    </row>
+    <row r="81" spans="3:7">
+      <c r="C81"/>
+      <c r="D81"/>
+      <c r="E81" s="75"/>
+      <c r="G81"/>
+    </row>
+    <row r="82" spans="3:7">
+      <c r="C82"/>
+      <c r="D82"/>
+      <c r="E82" s="75"/>
+      <c r="G82"/>
+    </row>
+    <row r="83" spans="3:7">
+      <c r="C83"/>
+      <c r="D83"/>
+      <c r="E83" s="75"/>
+      <c r="G83"/>
+    </row>
+    <row r="84" spans="3:7">
+      <c r="C84"/>
+      <c r="D84"/>
+      <c r="E84" s="75"/>
+      <c r="G84"/>
+    </row>
+    <row r="85" spans="3:7">
+      <c r="C85"/>
+      <c r="D85"/>
+      <c r="E85" s="75"/>
+      <c r="G85"/>
+    </row>
+    <row r="86" spans="3:7">
+      <c r="C86"/>
+      <c r="D86"/>
+      <c r="E86" s="75"/>
+      <c r="G86"/>
+    </row>
+    <row r="87" spans="3:7">
+      <c r="C87"/>
+      <c r="D87"/>
+      <c r="E87" s="75"/>
+      <c r="G87"/>
+    </row>
+    <row r="88" spans="3:7">
+      <c r="C88"/>
+      <c r="D88"/>
+      <c r="E88" s="75"/>
+      <c r="G88"/>
+    </row>
+    <row r="89" spans="3:7">
+      <c r="C89"/>
+      <c r="D89"/>
+      <c r="E89" s="75"/>
+      <c r="G89"/>
+    </row>
+    <row r="90" spans="3:7">
+      <c r="C90"/>
+      <c r="D90"/>
+      <c r="E90" s="75"/>
+      <c r="G90"/>
+    </row>
+    <row r="91" spans="3:7">
+      <c r="C91"/>
+      <c r="D91"/>
+      <c r="E91" s="75"/>
+      <c r="G91"/>
+    </row>
+    <row r="92" spans="3:7">
+      <c r="C92"/>
+      <c r="D92"/>
+      <c r="E92" s="75"/>
+      <c r="G92"/>
+    </row>
+    <row r="93" spans="3:7">
+      <c r="C93"/>
+      <c r="D93"/>
+      <c r="E93" s="75"/>
+      <c r="G93"/>
+    </row>
+    <row r="94" spans="3:7">
+      <c r="C94"/>
+      <c r="D94"/>
+      <c r="E94" s="75"/>
+      <c r="G94"/>
+    </row>
+    <row r="95" spans="3:7">
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="E95" s="75"/>
+      <c r="G95"/>
+    </row>
+    <row r="96" spans="3:7">
+      <c r="C96"/>
+      <c r="D96"/>
+      <c r="E96" s="75"/>
+      <c r="G96"/>
+    </row>
+    <row r="97" spans="3:7">
+      <c r="C97"/>
+      <c r="D97"/>
+      <c r="E97" s="75"/>
+      <c r="G97"/>
+    </row>
+    <row r="98" spans="3:7">
+      <c r="C98"/>
+      <c r="D98"/>
+      <c r="E98" s="75"/>
+      <c r="G98"/>
+    </row>
+    <row r="99" spans="3:7">
+      <c r="C99"/>
+      <c r="D99"/>
+      <c r="E99" s="75"/>
+      <c r="G99"/>
+    </row>
+    <row r="100" spans="3:7">
+      <c r="C100"/>
+      <c r="D100"/>
+      <c r="E100" s="75"/>
+      <c r="G100"/>
+    </row>
+    <row r="101" spans="3:7">
+      <c r="C101"/>
+      <c r="D101"/>
+      <c r="E101" s="75"/>
+      <c r="G101"/>
+    </row>
+    <row r="102" spans="3:7">
+      <c r="C102"/>
+      <c r="D102"/>
+      <c r="E102" s="75"/>
+      <c r="G102"/>
+    </row>
+    <row r="103" spans="3:7">
+      <c r="C103"/>
+      <c r="D103"/>
+      <c r="E103" s="75"/>
+      <c r="G103"/>
+    </row>
+    <row r="104" spans="3:7">
+      <c r="C104"/>
+      <c r="D104"/>
+      <c r="E104" s="75"/>
+      <c r="G104"/>
+    </row>
+    <row r="105" spans="3:7">
+      <c r="C105"/>
+      <c r="D105"/>
+      <c r="E105" s="75"/>
+      <c r="G105"/>
+    </row>
+    <row r="106" spans="3:7">
+      <c r="C106"/>
+      <c r="D106"/>
+      <c r="E106" s="75"/>
+      <c r="G106"/>
+    </row>
+    <row r="107" spans="3:7">
+      <c r="C107"/>
+      <c r="D107"/>
+      <c r="E107" s="75"/>
+      <c r="G107"/>
+    </row>
+    <row r="108" spans="3:7">
+      <c r="C108"/>
+      <c r="D108"/>
+      <c r="E108" s="75"/>
+      <c r="G108"/>
+    </row>
+    <row r="109" spans="3:7">
+      <c r="C109"/>
+      <c r="D109"/>
+      <c r="E109" s="75"/>
+      <c r="G109"/>
+    </row>
+    <row r="110" spans="3:7">
+      <c r="C110"/>
+      <c r="D110"/>
+      <c r="E110" s="75"/>
+      <c r="G110"/>
+    </row>
+    <row r="111" spans="3:7">
+      <c r="C111"/>
+      <c r="D111"/>
+      <c r="E111" s="75"/>
+      <c r="G111"/>
+    </row>
+    <row r="112" spans="3:7">
+      <c r="C112"/>
+      <c r="D112"/>
+      <c r="E112" s="75"/>
+      <c r="G112"/>
+    </row>
+    <row r="113" spans="3:7">
+      <c r="C113"/>
+      <c r="D113"/>
+      <c r="E113" s="75"/>
+      <c r="G113"/>
+    </row>
+    <row r="114" spans="3:7">
+      <c r="C114"/>
+      <c r="D114"/>
+      <c r="E114" s="75"/>
+      <c r="G114"/>
+    </row>
+    <row r="115" spans="3:7">
+      <c r="C115"/>
+      <c r="D115"/>
+      <c r="E115" s="75"/>
+      <c r="G115"/>
+    </row>
+    <row r="116" spans="3:7">
+      <c r="C116"/>
+      <c r="D116"/>
+      <c r="E116" s="75"/>
+      <c r="G116"/>
+    </row>
+    <row r="117" spans="3:7">
+      <c r="C117"/>
+      <c r="D117"/>
+      <c r="E117" s="75"/>
+      <c r="G117"/>
+    </row>
+    <row r="118" spans="3:7">
+      <c r="C118"/>
+      <c r="D118"/>
+      <c r="E118" s="75"/>
+      <c r="G118"/>
+    </row>
+    <row r="119" spans="3:7">
+      <c r="C119"/>
+      <c r="D119"/>
+      <c r="E119" s="75"/>
+      <c r="G119"/>
+    </row>
+    <row r="120" spans="3:7">
+      <c r="C120"/>
+      <c r="D120"/>
+      <c r="E120" s="75"/>
+      <c r="G120"/>
+    </row>
+    <row r="121" spans="3:7">
+      <c r="C121"/>
+      <c r="D121"/>
+      <c r="E121" s="75"/>
+      <c r="G121"/>
+    </row>
+    <row r="122" spans="3:7">
+      <c r="C122"/>
+      <c r="D122"/>
+      <c r="E122" s="75"/>
+      <c r="G122"/>
+    </row>
+    <row r="123" spans="3:7">
+      <c r="C123"/>
+      <c r="D123"/>
+      <c r="E123" s="75"/>
+      <c r="G123"/>
+    </row>
+    <row r="124" spans="3:7">
+      <c r="C124"/>
+      <c r="D124"/>
+      <c r="E124" s="75"/>
+      <c r="G124"/>
+    </row>
+    <row r="125" spans="3:7">
+      <c r="C125"/>
+      <c r="D125"/>
+      <c r="E125" s="75"/>
+      <c r="G125"/>
+    </row>
+    <row r="126" spans="3:7">
+      <c r="C126"/>
+      <c r="D126"/>
+      <c r="E126" s="75"/>
+      <c r="G126"/>
+    </row>
+    <row r="127" spans="3:7">
+      <c r="C127"/>
+      <c r="D127"/>
+      <c r="E127" s="75"/>
+      <c r="G127"/>
+    </row>
+    <row r="128" spans="3:7">
+      <c r="C128"/>
+      <c r="D128"/>
+      <c r="E128" s="75"/>
+      <c r="G128"/>
+    </row>
+    <row r="129" spans="3:7">
+      <c r="C129"/>
+      <c r="D129"/>
+      <c r="E129" s="75"/>
+      <c r="G129"/>
+    </row>
+    <row r="130" spans="3:7">
+      <c r="C130"/>
+      <c r="D130"/>
+      <c r="E130" s="75"/>
+      <c r="G130"/>
+    </row>
+    <row r="131" spans="3:7">
+      <c r="C131"/>
+      <c r="D131"/>
+      <c r="E131" s="75"/>
+      <c r="G131"/>
+    </row>
+    <row r="132" spans="3:7">
+      <c r="C132"/>
+      <c r="D132"/>
+      <c r="E132" s="75"/>
+      <c r="G132"/>
+    </row>
+    <row r="133" spans="3:7">
+      <c r="C133"/>
+      <c r="D133"/>
+      <c r="E133" s="75"/>
+      <c r="G133"/>
+    </row>
+    <row r="134" spans="3:7">
+      <c r="C134"/>
+      <c r="D134"/>
+      <c r="E134" s="75"/>
+      <c r="G134"/>
+    </row>
+    <row r="135" spans="3:7">
+      <c r="C135"/>
+      <c r="D135"/>
+      <c r="E135" s="75"/>
+      <c r="G135"/>
+    </row>
+    <row r="136" spans="3:7">
+      <c r="C136"/>
+      <c r="D136"/>
+      <c r="E136" s="75"/>
+      <c r="G136"/>
+    </row>
+    <row r="137" spans="3:7">
+      <c r="C137"/>
+      <c r="D137"/>
+      <c r="E137" s="75"/>
+      <c r="G137"/>
+    </row>
+    <row r="138" spans="3:7">
+      <c r="C138"/>
+      <c r="D138"/>
+      <c r="E138" s="75"/>
+      <c r="G138"/>
+    </row>
+    <row r="139" spans="3:7">
+      <c r="C139"/>
+      <c r="D139"/>
+      <c r="E139" s="75"/>
+      <c r="G139"/>
+    </row>
+    <row r="140" spans="3:7">
+      <c r="C140"/>
+      <c r="D140"/>
+      <c r="E140" s="75"/>
+      <c r="G140"/>
+    </row>
+    <row r="141" spans="3:7">
+      <c r="C141"/>
+      <c r="D141"/>
+      <c r="E141" s="75"/>
+      <c r="G141"/>
+    </row>
+    <row r="142" spans="3:7">
+      <c r="C142"/>
+      <c r="D142"/>
+      <c r="E142" s="75"/>
+      <c r="G142"/>
+    </row>
+    <row r="143" spans="3:7">
+      <c r="C143"/>
+      <c r="D143"/>
+      <c r="E143" s="75"/>
+      <c r="G143"/>
+    </row>
+    <row r="144" spans="3:7">
+      <c r="C144"/>
+      <c r="D144"/>
+      <c r="E144" s="75"/>
+      <c r="G144"/>
+    </row>
+    <row r="145" spans="3:7">
+      <c r="C145"/>
+      <c r="D145"/>
+      <c r="E145" s="75"/>
+      <c r="G145"/>
+    </row>
+    <row r="146" spans="3:7">
+      <c r="C146"/>
+      <c r="D146"/>
+      <c r="E146" s="75"/>
+      <c r="G146"/>
+    </row>
+    <row r="147" spans="3:7">
+      <c r="C147"/>
+      <c r="D147"/>
+      <c r="E147" s="75"/>
+      <c r="G147"/>
+    </row>
+    <row r="148" spans="3:7">
+      <c r="C148"/>
+      <c r="D148"/>
+      <c r="E148" s="75"/>
+      <c r="G148"/>
+    </row>
+    <row r="149" spans="3:7">
+      <c r="C149"/>
+      <c r="D149"/>
+      <c r="E149" s="75"/>
+      <c r="G149"/>
+    </row>
+    <row r="150" spans="3:7">
+      <c r="C150"/>
+      <c r="D150"/>
+      <c r="E150" s="75"/>
+      <c r="G150"/>
+    </row>
+    <row r="151" spans="3:7">
+      <c r="C151"/>
+      <c r="D151"/>
+      <c r="E151" s="75"/>
+      <c r="G151"/>
+    </row>
+    <row r="152" spans="3:7">
+      <c r="C152"/>
+      <c r="D152"/>
+      <c r="E152" s="75"/>
+      <c r="G152"/>
+    </row>
+    <row r="153" spans="3:7">
+      <c r="C153"/>
+      <c r="D153"/>
+      <c r="E153" s="75"/>
+      <c r="G153"/>
+    </row>
+    <row r="154" spans="3:7">
+      <c r="C154"/>
+      <c r="D154"/>
+      <c r="E154" s="75"/>
+      <c r="G154"/>
+    </row>
+    <row r="155" spans="3:7">
+      <c r="C155"/>
+      <c r="D155"/>
+      <c r="E155" s="75"/>
+      <c r="G155"/>
+    </row>
+    <row r="156" spans="3:7">
+      <c r="C156"/>
+      <c r="D156"/>
+      <c r="E156" s="75"/>
+      <c r="G156"/>
+    </row>
+    <row r="157" spans="3:7">
+      <c r="C157"/>
+      <c r="D157"/>
+      <c r="E157" s="75"/>
+      <c r="G157"/>
+    </row>
+    <row r="158" spans="3:7">
+      <c r="C158"/>
+      <c r="D158"/>
+      <c r="E158" s="75"/>
+      <c r="G158"/>
+    </row>
+    <row r="159" spans="3:7">
+      <c r="C159"/>
+      <c r="D159"/>
+      <c r="E159" s="75"/>
+      <c r="G159"/>
+    </row>
+    <row r="160" spans="3:7">
+      <c r="C160"/>
+      <c r="D160"/>
+      <c r="E160" s="75"/>
+      <c r="G160"/>
+    </row>
+    <row r="161" spans="3:7">
+      <c r="C161"/>
+      <c r="D161"/>
+      <c r="E161" s="75"/>
+      <c r="G161"/>
+    </row>
+    <row r="162" spans="3:7">
+      <c r="C162"/>
+      <c r="D162"/>
+      <c r="E162" s="75"/>
+      <c r="G162"/>
+    </row>
+    <row r="163" spans="3:7">
+      <c r="C163"/>
+      <c r="D163"/>
+      <c r="E163" s="75"/>
+      <c r="G163"/>
+    </row>
+    <row r="164" spans="3:7">
+      <c r="C164"/>
+      <c r="D164"/>
+      <c r="E164" s="75"/>
+      <c r="G164"/>
+    </row>
+    <row r="165" spans="3:7">
+      <c r="C165"/>
+      <c r="D165"/>
+      <c r="E165" s="75"/>
+      <c r="G165"/>
+    </row>
+    <row r="166" spans="3:7">
+      <c r="C166"/>
+      <c r="D166"/>
+      <c r="E166" s="75"/>
+      <c r="G166"/>
+    </row>
+    <row r="167" spans="3:7">
+      <c r="C167"/>
+      <c r="D167"/>
+      <c r="E167" s="75"/>
+      <c r="G167"/>
+    </row>
+    <row r="168" spans="3:7">
+      <c r="C168"/>
+      <c r="D168"/>
+      <c r="E168" s="75"/>
+      <c r="G168"/>
+    </row>
+    <row r="169" spans="3:7">
+      <c r="C169"/>
+      <c r="D169"/>
+      <c r="E169" s="75"/>
+      <c r="G169"/>
+    </row>
+    <row r="170" spans="3:7">
+      <c r="C170"/>
+      <c r="D170"/>
+      <c r="E170" s="75"/>
+      <c r="G170"/>
+    </row>
+    <row r="171" spans="3:7">
+      <c r="C171"/>
+      <c r="D171"/>
+      <c r="E171" s="75"/>
+      <c r="G171"/>
+    </row>
+    <row r="172" spans="3:7">
+      <c r="C172"/>
+      <c r="D172"/>
+      <c r="E172" s="75"/>
+      <c r="G172"/>
+    </row>
+    <row r="173" spans="3:7">
+      <c r="C173"/>
+      <c r="D173"/>
+      <c r="E173" s="75"/>
+      <c r="G173"/>
+    </row>
+    <row r="174" spans="3:7">
+      <c r="C174"/>
+      <c r="D174"/>
+      <c r="E174" s="75"/>
+      <c r="G174"/>
+    </row>
+    <row r="175" spans="3:7">
+      <c r="C175"/>
+      <c r="D175"/>
+      <c r="E175" s="75"/>
+      <c r="G175"/>
+    </row>
+    <row r="176" spans="3:7">
+      <c r="C176"/>
+      <c r="D176"/>
+      <c r="E176" s="75"/>
+      <c r="G176"/>
+    </row>
+    <row r="177" spans="3:7">
+      <c r="C177"/>
+      <c r="D177"/>
+      <c r="E177" s="75"/>
+      <c r="G177"/>
+    </row>
+    <row r="178" spans="3:7">
+      <c r="C178"/>
+      <c r="D178"/>
+      <c r="E178" s="76"/>
+      <c r="G178"/>
+    </row>
+    <row r="179" spans="3:7">
+      <c r="C179"/>
+      <c r="D179"/>
+      <c r="E179" s="76"/>
+      <c r="G179"/>
+    </row>
+    <row r="180" spans="3:7">
+      <c r="C180"/>
+      <c r="D180"/>
+      <c r="E180" s="76"/>
+      <c r="G180"/>
+    </row>
+    <row r="181" spans="3:7">
+      <c r="C181"/>
+      <c r="D181"/>
+      <c r="E181" s="76"/>
+      <c r="G181"/>
+    </row>
+    <row r="182" spans="3:7">
+      <c r="C182"/>
+      <c r="D182"/>
+      <c r="E182" s="76"/>
+      <c r="G182"/>
+    </row>
+    <row r="183" spans="3:7">
+      <c r="C183"/>
+      <c r="D183"/>
+      <c r="E183" s="74"/>
+      <c r="G183"/>
+    </row>
+    <row r="184" spans="3:7">
+      <c r="C184"/>
+      <c r="D184"/>
+      <c r="E184" s="74"/>
+      <c r="G184"/>
+    </row>
+    <row r="185" spans="3:7">
+      <c r="C185"/>
+      <c r="D185"/>
+      <c r="E185" s="74"/>
+      <c r="G185"/>
+    </row>
+    <row r="186" spans="3:7">
+      <c r="C186"/>
+      <c r="D186"/>
+      <c r="E186" s="78"/>
+      <c r="G186"/>
+    </row>
+    <row r="187" spans="3:7">
+      <c r="C187"/>
+      <c r="D187"/>
+      <c r="E187" s="78"/>
+      <c r="G187"/>
+    </row>
+    <row r="188" spans="3:7">
+      <c r="C188"/>
+      <c r="D188"/>
+      <c r="E188" s="78"/>
+      <c r="G188"/>
+    </row>
+    <row r="189" spans="3:7">
+      <c r="C189"/>
+      <c r="D189"/>
+      <c r="E189" s="78"/>
+      <c r="G189"/>
+    </row>
+    <row r="190" spans="3:7">
+      <c r="C190"/>
+      <c r="D190"/>
+      <c r="E190" s="78"/>
+      <c r="G190"/>
+    </row>
+    <row r="191" spans="3:7">
+      <c r="C191"/>
+      <c r="D191"/>
+      <c r="E191" s="78"/>
+      <c r="G191"/>
+    </row>
+    <row r="192" spans="3:7">
+      <c r="C192"/>
+      <c r="D192"/>
+      <c r="E192" s="78"/>
+      <c r="G192"/>
+    </row>
+    <row r="193" spans="3:7">
+      <c r="C193"/>
+      <c r="D193"/>
+      <c r="E193" s="78"/>
+      <c r="G193"/>
+    </row>
+    <row r="194" spans="3:7">
+      <c r="C194"/>
+      <c r="D194"/>
+      <c r="E194" s="78"/>
+      <c r="G194"/>
+    </row>
+    <row r="195" spans="3:7">
+      <c r="C195"/>
+      <c r="D195"/>
+      <c r="E195" s="78"/>
+      <c r="G195"/>
+    </row>
+    <row r="196" spans="3:7">
+      <c r="C196"/>
+      <c r="D196"/>
+      <c r="E196" s="78"/>
+      <c r="G196"/>
+    </row>
+    <row r="197" spans="3:7">
+      <c r="C197"/>
+      <c r="D197"/>
+      <c r="E197" s="78"/>
+      <c r="G197"/>
+    </row>
+    <row r="198" spans="3:7">
+      <c r="C198"/>
+      <c r="D198"/>
+      <c r="E198" s="78"/>
+      <c r="G198"/>
+    </row>
+    <row r="199" spans="3:7">
+      <c r="C199"/>
+      <c r="D199"/>
+      <c r="E199" s="78"/>
+      <c r="G199"/>
+    </row>
+    <row r="200" spans="3:7">
+      <c r="C200"/>
+      <c r="D200"/>
+      <c r="E200" s="78"/>
+      <c r="G200"/>
+    </row>
+    <row r="201" spans="3:7">
+      <c r="C201"/>
+      <c r="D201"/>
+      <c r="E201" s="78"/>
+      <c r="G201"/>
+    </row>
+    <row r="202" spans="3:7">
+      <c r="C202"/>
+      <c r="D202"/>
+      <c r="E202" s="78"/>
+      <c r="G202"/>
+    </row>
+    <row r="203" spans="3:7">
+      <c r="C203"/>
+      <c r="D203"/>
+      <c r="E203" s="78"/>
+      <c r="G203"/>
+    </row>
+    <row r="204" spans="3:7">
+      <c r="C204"/>
+      <c r="D204"/>
+      <c r="E204" s="78"/>
+      <c r="G204"/>
+    </row>
+    <row r="205" spans="3:7">
+      <c r="C205"/>
+      <c r="D205"/>
+      <c r="E205" s="78"/>
+      <c r="G205"/>
+    </row>
+    <row r="206" spans="3:7">
+      <c r="C206"/>
+      <c r="D206"/>
+      <c r="E206" s="78"/>
+      <c r="G206"/>
     </row>
   </sheetData>
-  <sortState ref="G1:G185">
-    <sortCondition ref="G1:G185"/>
-  </sortState>
   <dataValidations count="60">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Institutional review board (IRB) number" sqref="C2:D2 G124"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Parasite density (/uL) based on PCR" sqref="C42:D42 G164"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Parasite density (/uL) based on microscopy" sqref="C40:D40 G162"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for coma" sqref="C35:D35 G157"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Type of study sample collected from if &quot;other&quot; was chosen in 'Study type' field" sqref="D15 G183"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Other location where GPS coordinates were taken (other should be choosen in 'GPS location' field)" sqref="D13 G181"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="GPS coordinates of sample colleciton - longitude in decimal degrees (DD)" sqref="D10 G178"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="GPS coordinates of sample colleciton - latitude in decimal degrees (DD)" sqref="D11 G179"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Date of sample collected_x000a_Date in the format mm/dd/yyyy" sqref="C7:D7 G129"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Date of birth if available and known to be accurate_x000a_Date  in the format mm/dd/yyyy" sqref="C4:D4 G126"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="ICEMR regional center where sample was collected" sqref="C1:D1 G123"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for ARDS (Acute Respiratory Distress Syndrome)" sqref="C28:D28 G150"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for acute renal failure" sqref="C32:D32 G154"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for hypoglycemia" sqref="C31:D31 G153"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for generalized convulsions" sqref="C30:D30 G152"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for jaundice" sqref="C29:D29 G151"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for respiratory distress" sqref="C27:D27 G149"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for cerebral malaria" sqref="C26:D26 G148"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for severe anemia" sqref="C25:D25 G147"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Method used to measure temperature" sqref="C24:D24 G146"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="body temperature in °C" sqref="C23:D23 G145"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Duration of history of subjective fever in days" sqref="C22:D22 G144"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="History of subjective fever" sqref="C21:D21 G143"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="pregnancy status of study subject" sqref="C19:D19 G141"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="health status at time of physical examination" sqref="C18:D18 G140"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Was the patient hospitalized" sqref="C20:D20 G142"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Number of days between subsequent samples taken from the same individual" sqref="D17 G185"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Village/City/Town of sample collection" sqref="D9 G177"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Gender of study subject" sqref="C6:D6 G128"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="unique study paticipant ID number" sqref="C3:D3 G125"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Type of study sample collected from" sqref="D14 G182"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="specify original or follow up collection from same patient" sqref="D16 G184"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Location where the GPS coordinates were taken" sqref="D12 G180"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Age of participant in years" sqref="C5:D5 G127"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="PCR method used to detect asexual parasites" sqref="C43:D43 G165"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Results of PCR for detection of asexual parasites" sqref="C41:D41 G163"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Results of Microscopy (thin or think smear)" sqref="C39:D39 G161"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Type of RDT used" sqref="C38:D38 G160"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Rapid Diagnostic Test result" sqref="C37:D37 G159"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for fluid and electrolyte disturbances" sqref="C36:D36 G158"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for circulatory collapse" sqref="C34:D34 G156"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for abnormal bleeding" sqref="C33:D33 G155"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Informed consent for future use of samples" sqref="B61:D61 G122"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Informed consent for data collection and usage" sqref="B60:D60 G121"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Other molecular data available" sqref="B59:D59 G120"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data avaiable on immune responses" sqref="B58:D58 G119"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data available on parasite genetics" sqref="B57:D57 G118"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data available on host genetics" sqref="B56:D56 G117"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any other additional comments" sqref="B55:D55 G116"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Hemoglobin value (g/dL)" sqref="B54:D54 G115"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="P. knowlesi present" sqref="C53:D53 G175"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="P. vivax present" sqref="C52:D52 G174"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="P. ovale present" sqref="C51:D51 G173"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="P. malariae present" sqref="C50:D50 G172"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="P. falciparum present" sqref="C49:D49 G171"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Other method used to detect gametocytes (for example membrane feeding)" sqref="C48:D48 G170"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Method used to detect gametocytes" sqref="C47:D47 G169"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Gametocyte density(/uL) based on RT-PCR" sqref="C46:D46 G168"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Gametocyte density(/uL) based on microscopy" sqref="C45:D45 G167"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Gametocytes present" sqref="C44 G166"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Institutional review board (IRB) number" sqref="C2:D2 E124"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Parasite density (/uL) based on PCR" sqref="C42:D42 E164"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Parasite density (/uL) based on microscopy" sqref="C40:D40 E162"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for coma" sqref="C35:D35 E157"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Type of study sample collected from if &quot;other&quot; was chosen in 'Study type' field" sqref="D15 E183"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Other location where GPS coordinates were taken (other should be choosen in 'GPS location' field)" sqref="D13 E181"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="GPS coordinates of sample colleciton - longitude in decimal degrees (DD)" sqref="D10 E178"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="GPS coordinates of sample colleciton - latitude in decimal degrees (DD)" sqref="D11 E179"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Date of sample collected_x000a_Date in the format mm/dd/yyyy" sqref="C7:D7 E129"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Date of birth if available and known to be accurate_x000a_Date  in the format mm/dd/yyyy" sqref="C4:D4 E126"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="ICEMR regional center where sample was collected" sqref="C1:D1 E123"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for ARDS (Acute Respiratory Distress Syndrome)" sqref="C28:D28 E150"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for acute renal failure" sqref="C32:D32 E154"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for hypoglycemia" sqref="C31:D31 E153"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for generalized convulsions" sqref="C30:D30 E152"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for jaundice" sqref="C29:D29 E151"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for respiratory distress" sqref="C27:D27 E149"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for cerebral malaria" sqref="C26:D26 E148"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for severe anemia" sqref="C25:D25 E147"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Method used to measure temperature" sqref="C24:D24 E146"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="body temperature in °C" sqref="C23:D23 E145"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Duration of history of subjective fever in days" sqref="C22:D22 E144"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="History of subjective fever" sqref="C21:D21 E143"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="pregnancy status of study subject" sqref="C19:D19 E141"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="health status at time of physical examination" sqref="C18:D18 E140"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Was the patient hospitalized" sqref="C20:D20 E142"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Number of days between subsequent samples taken from the same individual" sqref="D17 E185"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Village/City/Town of sample collection" sqref="D9 E177"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Gender of study subject" sqref="C6:D6 E128"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="unique study paticipant ID number" sqref="C3:D3 E125"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Type of study sample collected from" sqref="D14 E182"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="specify original or follow up collection from same patient" sqref="D16 E184"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Location where the GPS coordinates were taken" sqref="D12 E180"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Age of participant in years" sqref="C5:D5 E127"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="PCR method used to detect asexual parasites" sqref="C43:D43 E165"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Results of PCR for detection of asexual parasites" sqref="C41:D41 E163"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Results of Microscopy (thin or think smear)" sqref="C39:D39 E161"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Type of RDT used" sqref="C38:D38 E160"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Rapid Diagnostic Test result" sqref="C37:D37 E159"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for fluid and electrolyte disturbances" sqref="C36:D36 E158"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for circulatory collapse" sqref="C34:D34 E156"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does the patient meet criteria for abnormal bleeding" sqref="C33:D33 E155"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Informed consent for future use of samples" sqref="B61:D61 E122"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Informed consent for data collection and usage" sqref="B60:D60 E121"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Other molecular data available" sqref="B59:D59 E120"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data avaiable on immune responses" sqref="B58:D58 E119"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data available on parasite genetics" sqref="B57:D57 E118"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data available on host genetics" sqref="B56:D56 E117"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any other additional comments" sqref="B55:D55 E116"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Hemoglobin value (g/dL)" sqref="B54:D54 E115"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="P. knowlesi present" sqref="C53:D53 E175"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="P. vivax present" sqref="C52:D52 E174"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="P. ovale present" sqref="C51:D51 E173"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="P. malariae present" sqref="C50:D50 E172"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="P. falciparum present" sqref="C49:D49 E171"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Other method used to detect gametocytes (for example membrane feeding)" sqref="C48:D48 E170"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Method used to detect gametocytes" sqref="C47:D47 E169"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Gametocyte density(/uL) based on RT-PCR" sqref="C46:D46 E168"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Gametocyte density(/uL) based on microscopy" sqref="C45:D45 E167"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Gametocytes present" sqref="C44 E166"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
add mapped ontology IRIs and IDs to ICEMR protein array terms
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@82759 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ICEMR/ICEMR protein array/ICEMR submission form v3 ontology mapping.xlsx
+++ b/Load/src/ontology/ICEMR/ICEMR protein array/ICEMR submission form v3 ontology mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26423"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14380"/>
+    <workbookView xWindow="2200" yWindow="2920" windowWidth="30780" windowHeight="14800"/>
   </bookViews>
   <sheets>
     <sheet name="terms" sheetId="5" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1737" uniqueCount="917">
   <si>
     <t>uniqueid</t>
   </si>
@@ -2401,9 +2401,6 @@
     <t>information on availability of molecular data</t>
   </si>
   <si>
-    <t xml:space="preserve">information on original or follow up specimen collection </t>
-  </si>
-  <si>
     <t>information on informed consent for data collection and usage</t>
   </si>
   <si>
@@ -2414,9 +2411,6 @@
   </si>
   <si>
     <t>location where GPS coordinates were taken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">information on availabilty of host genetics data </t>
   </si>
   <si>
     <t>presence of Plasmodium knowlesi</t>
@@ -2531,6 +2525,324 @@
   <si>
     <t>tagged using inSubset: ICEMR protein array</t>
   </si>
+  <si>
+    <t>information on original or follow up specimen collection</t>
+  </si>
+  <si>
+    <t>information on availabilty of host genetics data</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000534</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000513</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000514</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000515</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000516</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000518</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000525</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000553</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000528</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000526</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000527</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000519</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000529</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000530</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000531</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000532</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000535</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000520</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000521</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000522</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000546</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000550</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000552</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000547</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000548</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000551</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000549</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000538</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000537</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000536</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000533</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000539</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000540</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000523</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000541</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UBERON_0009097</t>
+  </si>
+  <si>
+    <t>mapped ontology term ID</t>
+  </si>
+  <si>
+    <t>HP_0001892</t>
+  </si>
+  <si>
+    <t>EUPATH_0000113</t>
+  </si>
+  <si>
+    <t>DOID_11394</t>
+  </si>
+  <si>
+    <t>EUPATH_0000513</t>
+  </si>
+  <si>
+    <t>DOID_14069</t>
+  </si>
+  <si>
+    <t>OGMS_0000014</t>
+  </si>
+  <si>
+    <t>EUPATH_0000514</t>
+  </si>
+  <si>
+    <t>HP_0001259</t>
+  </si>
+  <si>
+    <t>OBI_0001898</t>
+  </si>
+  <si>
+    <t>SYMP_0000596</t>
+  </si>
+  <si>
+    <t>EUPATH_0000515</t>
+  </si>
+  <si>
+    <t>EUPATH_0000032</t>
+  </si>
+  <si>
+    <t>EUPATH_0000516</t>
+  </si>
+  <si>
+    <t>EUPATH_0000518</t>
+  </si>
+  <si>
+    <t>EUPATH_0000097</t>
+  </si>
+  <si>
+    <t>EUPATH_0000414</t>
+  </si>
+  <si>
+    <t>EUPATH_0000525</t>
+  </si>
+  <si>
+    <t>EUPATH_0000553</t>
+  </si>
+  <si>
+    <t>EUPATH_0000528</t>
+  </si>
+  <si>
+    <t>EUPATH_0000526</t>
+  </si>
+  <si>
+    <t>EUPATH_0000527</t>
+  </si>
+  <si>
+    <t>EUPATH_0000519</t>
+  </si>
+  <si>
+    <t>EUPATH_0000529</t>
+  </si>
+  <si>
+    <t>EUPATH_0000096</t>
+  </si>
+  <si>
+    <t>OBI_0001620</t>
+  </si>
+  <si>
+    <t>EUPATH_0000530</t>
+  </si>
+  <si>
+    <t>OBI_0001621</t>
+  </si>
+  <si>
+    <t>OGMS_0000073</t>
+  </si>
+  <si>
+    <t>EUPATH_0000047</t>
+  </si>
+  <si>
+    <t>EUPATH_0000308</t>
+  </si>
+  <si>
+    <t>EUPATH_0000531</t>
+  </si>
+  <si>
+    <t>DOID_9993</t>
+  </si>
+  <si>
+    <t>EUPATH_0000532</t>
+  </si>
+  <si>
+    <t>OBI_0000810</t>
+  </si>
+  <si>
+    <t>EUPATH_0000535</t>
+  </si>
+  <si>
+    <t>HP_0000952</t>
+  </si>
+  <si>
+    <t>EUPATH_0000520</t>
+  </si>
+  <si>
+    <t>OGMS_0000018</t>
+  </si>
+  <si>
+    <t>EUPATH_0000521</t>
+  </si>
+  <si>
+    <t>EUPATH_0000048</t>
+  </si>
+  <si>
+    <t>EUPATH_0000309</t>
+  </si>
+  <si>
+    <t>EUPATH_0000534</t>
+  </si>
+  <si>
+    <t>EUPATH_0000522</t>
+  </si>
+  <si>
+    <t>EUPATH_0000546</t>
+  </si>
+  <si>
+    <t>EUPATH_0000550</t>
+  </si>
+  <si>
+    <t>EUPATH_0000552</t>
+  </si>
+  <si>
+    <t>EUPATH_0000547</t>
+  </si>
+  <si>
+    <t>EUPATH_0000548</t>
+  </si>
+  <si>
+    <t>EUPATH_0000551</t>
+  </si>
+  <si>
+    <t>EUPATH_0000549</t>
+  </si>
+  <si>
+    <t>EUPATH_0000538</t>
+  </si>
+  <si>
+    <t>EUPATH_0000537</t>
+  </si>
+  <si>
+    <t>EUPATH_0000536</t>
+  </si>
+  <si>
+    <t>EUPATH_0000533</t>
+  </si>
+  <si>
+    <t>EUPATH_0000539</t>
+  </si>
+  <si>
+    <t>EUPATH_0000540</t>
+  </si>
+  <si>
+    <t>EUPATH_0000523</t>
+  </si>
+  <si>
+    <t>EUPATH_0000541</t>
+  </si>
+  <si>
+    <t>HP_0000083</t>
+  </si>
+  <si>
+    <t>HP_0002098</t>
+  </si>
+  <si>
+    <t>OBI_0001616</t>
+  </si>
+  <si>
+    <t>EUPATH_0000215</t>
+  </si>
+  <si>
+    <t>OBI_0000659</t>
+  </si>
+  <si>
+    <t>OBI_0500000</t>
+  </si>
+  <si>
+    <t>EUPATH_0000095</t>
+  </si>
+  <si>
+    <t>EUPATH_0000110</t>
+  </si>
+  <si>
+    <t>SNOMEDCT_27942005</t>
+  </si>
 </sst>
 </file>
 
@@ -2540,9 +2852,16 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2699,6 +3018,12 @@
     <font>
       <sz val="11"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF366092"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -3030,270 +3355,316 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="195">
+  <cellStyleXfs count="241">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -3303,162 +3674,96 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="17" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="17" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="17" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="17" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="17" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="17" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3476,50 +3781,117 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="195">
+  <cellStyles count="241">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3621,6 +3993,31 @@
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
@@ -3713,6 +4110,27 @@
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -4022,25 +4440,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I90"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="E57" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="33.1640625" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="51.33203125" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" customWidth="1"/>
-    <col min="8" max="8" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="41.83203125" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" customWidth="1"/>
+    <col min="6" max="6" width="42.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19.5" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" customWidth="1"/>
+    <col min="9" max="9" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
+    <row r="1" spans="1:10" ht="15">
       <c r="A1" s="54" t="s">
         <v>480</v>
       </c>
@@ -4060,16 +4479,19 @@
         <v>485</v>
       </c>
       <c r="G1" s="54" t="s">
-        <v>812</v>
+        <v>849</v>
       </c>
       <c r="H1" s="54" t="s">
+        <v>810</v>
+      </c>
+      <c r="I1" s="54" t="s">
         <v>486</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="J1" s="55" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15">
+    <row r="2" spans="1:10" ht="15">
       <c r="A2" t="s">
         <v>430</v>
       </c>
@@ -4089,16 +4511,19 @@
         <v>430</v>
       </c>
       <c r="G2" t="s">
+        <v>850</v>
+      </c>
+      <c r="H2" t="s">
         <v>694</v>
       </c>
-      <c r="H2" t="s">
-        <v>797</v>
-      </c>
-      <c r="I2" s="56" t="s">
+      <c r="I2" t="s">
+        <v>795</v>
+      </c>
+      <c r="J2" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15">
+    <row r="3" spans="1:10" ht="15">
       <c r="A3" t="s">
         <v>400</v>
       </c>
@@ -4118,16 +4543,19 @@
         <v>753</v>
       </c>
       <c r="G3" t="s">
+        <v>851</v>
+      </c>
+      <c r="H3" t="s">
         <v>694</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>495</v>
       </c>
-      <c r="I3" s="56" t="s">
+      <c r="J3" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15">
+    <row r="4" spans="1:10" ht="15">
       <c r="A4" t="s">
         <v>429</v>
       </c>
@@ -4147,16 +4575,19 @@
         <v>498</v>
       </c>
       <c r="G4" t="s">
+        <v>852</v>
+      </c>
+      <c r="H4" t="s">
         <v>694</v>
       </c>
-      <c r="H4" t="s">
-        <v>797</v>
-      </c>
-      <c r="I4" s="56" t="s">
+      <c r="I4" t="s">
+        <v>795</v>
+      </c>
+      <c r="J4" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15">
+    <row r="5" spans="1:10" ht="15">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -4169,20 +4600,26 @@
       <c r="D5" t="s">
         <v>500</v>
       </c>
+      <c r="E5" s="66" t="s">
+        <v>814</v>
+      </c>
       <c r="F5" s="66" t="s">
         <v>778</v>
       </c>
-      <c r="G5" s="66" t="s">
+      <c r="G5" t="s">
+        <v>853</v>
+      </c>
+      <c r="H5" s="66" t="s">
         <v>694</v>
       </c>
-      <c r="H5" s="66" t="s">
+      <c r="I5" s="66" t="s">
         <v>501</v>
       </c>
-      <c r="I5" s="56" t="s">
+      <c r="J5" s="56" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15">
+    <row r="6" spans="1:10" ht="15">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -4202,16 +4639,19 @@
         <v>505</v>
       </c>
       <c r="G6" t="s">
+        <v>854</v>
+      </c>
+      <c r="H6" t="s">
         <v>694</v>
       </c>
-      <c r="H6" s="58" t="s">
+      <c r="I6" s="58" t="s">
         <v>495</v>
       </c>
-      <c r="I6" s="56" t="s">
+      <c r="J6" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15">
+    <row r="7" spans="1:10" ht="15">
       <c r="A7" t="s">
         <v>417</v>
       </c>
@@ -4231,16 +4671,19 @@
         <v>508</v>
       </c>
       <c r="G7" t="s">
+        <v>855</v>
+      </c>
+      <c r="H7" t="s">
         <v>694</v>
       </c>
-      <c r="H7" s="58" t="s">
+      <c r="I7" s="58" t="s">
         <v>509</v>
       </c>
-      <c r="I7" s="56" t="s">
+      <c r="J7" s="56" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15">
+    <row r="8" spans="1:10" ht="15">
       <c r="A8" t="s">
         <v>414</v>
       </c>
@@ -4253,20 +4696,26 @@
       <c r="D8" t="s">
         <v>512</v>
       </c>
+      <c r="E8" s="66" t="s">
+        <v>815</v>
+      </c>
       <c r="F8" s="66" t="s">
-        <v>779</v>
-      </c>
-      <c r="G8" s="66" t="s">
+        <v>811</v>
+      </c>
+      <c r="G8" t="s">
+        <v>856</v>
+      </c>
+      <c r="H8" s="66" t="s">
         <v>694</v>
       </c>
-      <c r="H8" s="66" t="s">
+      <c r="I8" s="66" t="s">
         <v>501</v>
       </c>
-      <c r="I8" s="56" t="s">
+      <c r="J8" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15">
+    <row r="9" spans="1:10" ht="15">
       <c r="A9" t="s">
         <v>468</v>
       </c>
@@ -4285,17 +4734,20 @@
       <c r="F9" s="56" t="s">
         <v>468</v>
       </c>
-      <c r="G9" s="56" t="s">
+      <c r="G9" t="s">
+        <v>857</v>
+      </c>
+      <c r="H9" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H9" t="s">
-        <v>797</v>
-      </c>
-      <c r="I9" s="56" t="s">
+      <c r="I9" t="s">
+        <v>795</v>
+      </c>
+      <c r="J9" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15">
+    <row r="10" spans="1:10" ht="15">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -4314,17 +4766,20 @@
       <c r="F10" s="56" t="s">
         <v>518</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" t="s">
+        <v>858</v>
+      </c>
+      <c r="H10" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H10" s="58" t="s">
+      <c r="I10" s="58" t="s">
         <v>519</v>
       </c>
-      <c r="I10" s="56" t="s">
+      <c r="J10" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15">
+    <row r="11" spans="1:10" ht="15">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -4343,17 +4798,20 @@
       <c r="F11" s="56" t="s">
         <v>522</v>
       </c>
-      <c r="G11" s="56" t="s">
+      <c r="G11" t="s">
+        <v>859</v>
+      </c>
+      <c r="H11" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H11" s="58" t="s">
+      <c r="I11" s="58" t="s">
         <v>495</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="J11" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15">
+    <row r="12" spans="1:10" ht="15">
       <c r="A12" t="s">
         <v>401</v>
       </c>
@@ -4372,17 +4830,20 @@
       <c r="F12" s="56" t="s">
         <v>765</v>
       </c>
-      <c r="G12" s="56" t="s">
+      <c r="G12" t="s">
+        <v>523</v>
+      </c>
+      <c r="H12" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H12" s="58" t="s">
+      <c r="I12" s="58" t="s">
         <v>525</v>
       </c>
-      <c r="I12" s="56" t="s">
+      <c r="J12" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15">
+    <row r="13" spans="1:10" ht="15">
       <c r="A13" t="s">
         <v>452</v>
       </c>
@@ -4395,20 +4856,26 @@
       <c r="D13" t="s">
         <v>528</v>
       </c>
+      <c r="E13" s="66" t="s">
+        <v>816</v>
+      </c>
       <c r="F13" s="66" t="s">
-        <v>780</v>
-      </c>
-      <c r="G13" s="66" t="s">
+        <v>779</v>
+      </c>
+      <c r="G13" t="s">
+        <v>860</v>
+      </c>
+      <c r="H13" s="66" t="s">
         <v>694</v>
       </c>
-      <c r="H13" s="67" t="s">
+      <c r="I13" s="67" t="s">
         <v>501</v>
       </c>
-      <c r="I13" s="56" t="s">
+      <c r="J13" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15">
+    <row r="14" spans="1:10" ht="15">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -4427,17 +4894,20 @@
       <c r="F14" s="56" t="s">
         <v>532</v>
       </c>
-      <c r="G14" s="56" t="s">
+      <c r="G14" t="s">
+        <v>861</v>
+      </c>
+      <c r="H14" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>533</v>
       </c>
-      <c r="I14" s="56" t="s">
+      <c r="J14" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15">
+    <row r="15" spans="1:10" ht="15">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -4456,17 +4926,20 @@
       <c r="F15" t="s">
         <v>768</v>
       </c>
-      <c r="G15" s="56" t="s">
+      <c r="G15" t="s">
+        <v>534</v>
+      </c>
+      <c r="H15" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>537</v>
       </c>
-      <c r="I15" s="56" t="s">
+      <c r="J15" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15">
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" t="s">
         <v>431</v>
       </c>
@@ -4479,21 +4952,26 @@
       <c r="D16" t="s">
         <v>490</v>
       </c>
-      <c r="E16" s="59"/>
+      <c r="E16" s="66" t="s">
+        <v>817</v>
+      </c>
       <c r="F16" s="67" t="s">
         <v>431</v>
       </c>
-      <c r="G16" s="67" t="s">
+      <c r="G16" t="s">
+        <v>862</v>
+      </c>
+      <c r="H16" s="67" t="s">
         <v>694</v>
       </c>
-      <c r="H16" s="67" t="s">
+      <c r="I16" s="67" t="s">
         <v>540</v>
       </c>
-      <c r="I16" s="56" t="s">
+      <c r="J16" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15">
+    <row r="17" spans="1:10" ht="15">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -4506,21 +4984,26 @@
       <c r="D17" t="s">
         <v>542</v>
       </c>
-      <c r="E17" s="59"/>
+      <c r="E17" s="66" t="s">
+        <v>818</v>
+      </c>
       <c r="F17" s="66" t="s">
-        <v>781</v>
-      </c>
-      <c r="G17" s="66" t="s">
+        <v>780</v>
+      </c>
+      <c r="G17" t="s">
+        <v>863</v>
+      </c>
+      <c r="H17" s="66" t="s">
         <v>694</v>
       </c>
-      <c r="H17" s="67" t="s">
+      <c r="I17" s="67" t="s">
         <v>543</v>
       </c>
-      <c r="I17" s="56" t="s">
+      <c r="J17" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15">
+    <row r="18" spans="1:10" ht="15">
       <c r="A18" s="26" t="s">
         <v>419</v>
       </c>
@@ -4539,17 +5022,20 @@
       <c r="F18" t="s">
         <v>546</v>
       </c>
-      <c r="G18" s="56" t="s">
+      <c r="G18" t="s">
+        <v>864</v>
+      </c>
+      <c r="H18" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>547</v>
       </c>
-      <c r="I18" s="56" t="s">
+      <c r="J18" s="56" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15">
+    <row r="19" spans="1:10" ht="15">
       <c r="A19" t="s">
         <v>421</v>
       </c>
@@ -4563,20 +5049,23 @@
         <v>544</v>
       </c>
       <c r="E19" s="56" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="F19" s="56" t="s">
         <v>754</v>
       </c>
-      <c r="G19" s="56" t="s">
+      <c r="G19" t="s">
+        <v>865</v>
+      </c>
+      <c r="H19" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H19" s="67"/>
-      <c r="I19" s="56" t="s">
+      <c r="I19" s="67"/>
+      <c r="J19" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15">
+    <row r="20" spans="1:10" ht="15">
       <c r="A20" t="s">
         <v>415</v>
       </c>
@@ -4589,20 +5078,26 @@
       <c r="D20" t="s">
         <v>512</v>
       </c>
+      <c r="E20" s="66" t="s">
+        <v>819</v>
+      </c>
       <c r="F20" s="67" t="s">
-        <v>810</v>
-      </c>
-      <c r="G20" s="67" t="s">
+        <v>808</v>
+      </c>
+      <c r="G20" t="s">
+        <v>866</v>
+      </c>
+      <c r="H20" s="67" t="s">
         <v>694</v>
       </c>
-      <c r="H20" s="67" t="s">
+      <c r="I20" s="67" t="s">
         <v>552</v>
       </c>
-      <c r="I20" s="56" t="s">
+      <c r="J20" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15">
+    <row r="21" spans="1:10" ht="15">
       <c r="A21" t="s">
         <v>453</v>
       </c>
@@ -4615,20 +5110,26 @@
       <c r="D21" t="s">
         <v>528</v>
       </c>
+      <c r="E21" s="66" t="s">
+        <v>820</v>
+      </c>
       <c r="F21" s="67" t="s">
-        <v>782</v>
-      </c>
-      <c r="G21" s="67" t="s">
+        <v>781</v>
+      </c>
+      <c r="G21" t="s">
+        <v>867</v>
+      </c>
+      <c r="H21" s="67" t="s">
         <v>694</v>
       </c>
-      <c r="H21" s="67" t="s">
+      <c r="I21" s="67" t="s">
         <v>501</v>
       </c>
-      <c r="I21" s="56" t="s">
+      <c r="J21" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15">
+    <row r="22" spans="1:10" ht="15">
       <c r="A22" s="26" t="s">
         <v>433</v>
       </c>
@@ -4641,20 +5142,26 @@
       <c r="D22" t="s">
         <v>516</v>
       </c>
+      <c r="E22" s="66" t="s">
+        <v>821</v>
+      </c>
       <c r="F22" s="67" t="s">
         <v>568</v>
       </c>
-      <c r="G22" s="67" t="s">
+      <c r="G22" t="s">
+        <v>868</v>
+      </c>
+      <c r="H22" s="67" t="s">
         <v>694</v>
       </c>
-      <c r="H22" s="66" t="s">
+      <c r="I22" s="66" t="s">
         <v>569</v>
       </c>
-      <c r="I22" s="56" t="s">
+      <c r="J22" s="56" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15">
+    <row r="23" spans="1:10" ht="15">
       <c r="A23" t="s">
         <v>441</v>
       </c>
@@ -4667,20 +5174,26 @@
       <c r="D23" t="s">
         <v>557</v>
       </c>
+      <c r="E23" s="66" t="s">
+        <v>822</v>
+      </c>
       <c r="F23" s="67" t="s">
         <v>558</v>
       </c>
-      <c r="G23" s="67" t="s">
+      <c r="G23" t="s">
+        <v>869</v>
+      </c>
+      <c r="H23" s="67" t="s">
         <v>694</v>
       </c>
-      <c r="H23" s="67" t="s">
+      <c r="I23" s="67" t="s">
         <v>559</v>
       </c>
-      <c r="I23" s="56" t="s">
+      <c r="J23" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15">
+    <row r="24" spans="1:10" ht="15">
       <c r="A24" t="s">
         <v>442</v>
       </c>
@@ -4693,20 +5206,26 @@
       <c r="D24" t="s">
         <v>557</v>
       </c>
+      <c r="E24" s="66" t="s">
+        <v>823</v>
+      </c>
       <c r="F24" s="67" t="s">
         <v>562</v>
       </c>
-      <c r="G24" s="67" t="s">
+      <c r="G24" t="s">
+        <v>870</v>
+      </c>
+      <c r="H24" s="67" t="s">
         <v>694</v>
       </c>
-      <c r="H24" s="67" t="s">
+      <c r="I24" s="67" t="s">
         <v>559</v>
       </c>
-      <c r="I24" s="56" t="s">
+      <c r="J24" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15">
+    <row r="25" spans="1:10" ht="15">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -4719,20 +5238,26 @@
       <c r="D25" t="s">
         <v>557</v>
       </c>
+      <c r="E25" s="66" t="s">
+        <v>824</v>
+      </c>
       <c r="F25" s="67" t="s">
         <v>564</v>
       </c>
-      <c r="G25" s="67" t="s">
+      <c r="G25" t="s">
+        <v>871</v>
+      </c>
+      <c r="H25" s="67" t="s">
         <v>694</v>
       </c>
-      <c r="H25" s="67" t="s">
+      <c r="I25" s="67" t="s">
         <v>565</v>
       </c>
-      <c r="I25" s="56" t="s">
+      <c r="J25" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15">
+    <row r="26" spans="1:10" ht="15">
       <c r="A26" t="s">
         <v>443</v>
       </c>
@@ -4745,20 +5270,26 @@
       <c r="D26" t="s">
         <v>557</v>
       </c>
+      <c r="E26" s="66" t="s">
+        <v>825</v>
+      </c>
       <c r="F26" s="67" t="s">
         <v>755</v>
       </c>
-      <c r="G26" s="67" t="s">
+      <c r="G26" t="s">
+        <v>872</v>
+      </c>
+      <c r="H26" s="67" t="s">
         <v>694</v>
       </c>
-      <c r="H26" s="67" t="s">
+      <c r="I26" s="67" t="s">
         <v>756</v>
       </c>
-      <c r="I26" s="56" t="s">
+      <c r="J26" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15">
+    <row r="27" spans="1:10" ht="15">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -4771,14 +5302,14 @@
       <c r="D27" t="s">
         <v>500</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>573</v>
       </c>
-      <c r="I27" s="56" t="s">
+      <c r="J27" s="56" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15">
+    <row r="28" spans="1:10" ht="15">
       <c r="A28" t="s">
         <v>403</v>
       </c>
@@ -4797,17 +5328,20 @@
       <c r="F28" t="s">
         <v>575</v>
       </c>
-      <c r="G28" s="56" t="s">
+      <c r="G28" t="s">
+        <v>873</v>
+      </c>
+      <c r="H28" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>495</v>
       </c>
-      <c r="I28" s="56" t="s">
+      <c r="J28" s="56" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15">
+    <row r="29" spans="1:10" ht="15">
       <c r="A29" t="s">
         <v>411</v>
       </c>
@@ -4826,17 +5360,20 @@
       <c r="F29" s="56" t="s">
         <v>579</v>
       </c>
-      <c r="G29" s="56" t="s">
+      <c r="G29" t="s">
+        <v>874</v>
+      </c>
+      <c r="H29" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>495</v>
       </c>
-      <c r="I29" s="56" t="s">
+      <c r="J29" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15">
+    <row r="30" spans="1:10" ht="15">
       <c r="A30" t="s">
         <v>404</v>
       </c>
@@ -4849,21 +5386,26 @@
       <c r="D30" t="s">
         <v>524</v>
       </c>
-      <c r="E30" s="56"/>
+      <c r="E30" s="66" t="s">
+        <v>826</v>
+      </c>
       <c r="F30" s="66" t="s">
-        <v>783</v>
-      </c>
-      <c r="G30" s="66" t="s">
+        <v>782</v>
+      </c>
+      <c r="G30" t="s">
+        <v>875</v>
+      </c>
+      <c r="H30" s="66" t="s">
         <v>694</v>
       </c>
-      <c r="H30" s="67" t="s">
+      <c r="I30" s="67" t="s">
         <v>759</v>
       </c>
-      <c r="I30" s="56" t="s">
+      <c r="J30" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15">
+    <row r="31" spans="1:10" ht="15">
       <c r="A31" t="s">
         <v>410</v>
       </c>
@@ -4882,17 +5424,20 @@
       <c r="F31" s="56" t="s">
         <v>585</v>
       </c>
-      <c r="G31" s="56" t="s">
+      <c r="G31" t="s">
+        <v>876</v>
+      </c>
+      <c r="H31" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>495</v>
       </c>
-      <c r="I31" s="56" t="s">
+      <c r="J31" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15">
+    <row r="32" spans="1:10" ht="15">
       <c r="A32" t="s">
         <v>408</v>
       </c>
@@ -4908,14 +5453,15 @@
       <c r="E32" s="59"/>
       <c r="F32" s="59"/>
       <c r="G32" s="59"/>
-      <c r="H32" t="s">
+      <c r="H32" s="59"/>
+      <c r="I32" t="s">
         <v>588</v>
       </c>
-      <c r="I32" s="56" t="s">
+      <c r="J32" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15">
+    <row r="33" spans="1:10" ht="15">
       <c r="A33" t="s">
         <v>416</v>
       </c>
@@ -4934,17 +5480,20 @@
       <c r="F33" s="56" t="s">
         <v>593</v>
       </c>
-      <c r="G33" s="56" t="s">
+      <c r="G33" t="s">
+        <v>877</v>
+      </c>
+      <c r="H33" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>495</v>
       </c>
-      <c r="I33" s="56" t="s">
+      <c r="J33" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15">
+    <row r="34" spans="1:10" ht="15">
       <c r="A34" t="s">
         <v>447</v>
       </c>
@@ -4963,17 +5512,20 @@
       <c r="F34" s="56" t="s">
         <v>597</v>
       </c>
-      <c r="G34" s="56" t="s">
+      <c r="G34" t="s">
+        <v>878</v>
+      </c>
+      <c r="H34" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>495</v>
       </c>
-      <c r="I34" s="56" t="s">
+      <c r="J34" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15">
+    <row r="35" spans="1:10" ht="15">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -4992,17 +5544,20 @@
       <c r="F35" t="s">
         <v>600</v>
       </c>
-      <c r="G35" s="67" t="s">
+      <c r="G35" t="s">
+        <v>879</v>
+      </c>
+      <c r="H35" s="67" t="s">
         <v>694</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>495</v>
       </c>
-      <c r="I35" s="56" t="s">
+      <c r="J35" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15">
+    <row r="36" spans="1:10" ht="15">
       <c r="A36" t="s">
         <v>449</v>
       </c>
@@ -5015,20 +5570,26 @@
       <c r="D36" t="s">
         <v>499</v>
       </c>
+      <c r="E36" s="66" t="s">
+        <v>827</v>
+      </c>
       <c r="F36" s="66" t="s">
-        <v>784</v>
-      </c>
-      <c r="G36" s="66" t="s">
+        <v>812</v>
+      </c>
+      <c r="G36" t="s">
+        <v>880</v>
+      </c>
+      <c r="H36" s="66" t="s">
         <v>694</v>
       </c>
-      <c r="H36" s="67" t="s">
+      <c r="I36" s="67" t="s">
         <v>501</v>
       </c>
-      <c r="I36" s="56" t="s">
+      <c r="J36" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15">
+    <row r="37" spans="1:10" ht="15">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -5047,17 +5608,20 @@
       <c r="F37" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="G37" s="56" t="s">
+      <c r="G37" t="s">
+        <v>881</v>
+      </c>
+      <c r="H37" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>495</v>
       </c>
-      <c r="I37" s="56" t="s">
+      <c r="J37" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15">
+    <row r="38" spans="1:10" ht="15">
       <c r="A38" t="s">
         <v>450</v>
       </c>
@@ -5070,21 +5634,26 @@
       <c r="D38" t="s">
         <v>499</v>
       </c>
-      <c r="E38" s="59"/>
+      <c r="E38" s="66" t="s">
+        <v>828</v>
+      </c>
       <c r="F38" s="66" t="s">
-        <v>787</v>
-      </c>
-      <c r="G38" s="66" t="s">
+        <v>785</v>
+      </c>
+      <c r="G38" t="s">
+        <v>882</v>
+      </c>
+      <c r="H38" s="66" t="s">
         <v>694</v>
       </c>
-      <c r="H38" s="67" t="s">
+      <c r="I38" s="67" t="s">
         <v>501</v>
       </c>
-      <c r="I38" s="56" t="s">
+      <c r="J38" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15">
+    <row r="39" spans="1:10" ht="15">
       <c r="A39" t="s">
         <v>405</v>
       </c>
@@ -5097,14 +5666,14 @@
       <c r="D39" t="s">
         <v>536</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>607</v>
       </c>
-      <c r="I39" s="56" t="s">
+      <c r="J39" s="56" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15">
+    <row r="40" spans="1:10" ht="15">
       <c r="A40" t="s">
         <v>135</v>
       </c>
@@ -5123,17 +5692,20 @@
       <c r="F40" s="56" t="s">
         <v>609</v>
       </c>
-      <c r="G40" s="56" t="s">
+      <c r="G40" t="s">
+        <v>883</v>
+      </c>
+      <c r="H40" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H40" t="s">
-        <v>797</v>
-      </c>
-      <c r="I40" s="56" t="s">
+      <c r="I40" t="s">
+        <v>795</v>
+      </c>
+      <c r="J40" s="56" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15">
+    <row r="41" spans="1:10" ht="15">
       <c r="A41" t="s">
         <v>474</v>
       </c>
@@ -5146,21 +5718,26 @@
       <c r="D41" t="s">
         <v>494</v>
       </c>
-      <c r="E41" s="59"/>
+      <c r="E41" s="66" t="s">
+        <v>829</v>
+      </c>
       <c r="F41" s="66" t="s">
         <v>474</v>
       </c>
-      <c r="G41" s="66" t="s">
+      <c r="G41" t="s">
+        <v>884</v>
+      </c>
+      <c r="H41" s="66" t="s">
         <v>694</v>
       </c>
-      <c r="H41" s="67" t="s">
+      <c r="I41" s="67" t="s">
         <v>612</v>
       </c>
-      <c r="I41" s="56" t="s">
+      <c r="J41" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15">
+    <row r="42" spans="1:10" ht="15">
       <c r="A42" t="s">
         <v>73</v>
       </c>
@@ -5179,17 +5756,20 @@
       <c r="F42" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="G42" s="56" t="s">
+      <c r="G42" t="s">
+        <v>885</v>
+      </c>
+      <c r="H42" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>495</v>
       </c>
-      <c r="I42" s="56" t="s">
+      <c r="J42" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15">
+    <row r="43" spans="1:10" ht="15">
       <c r="A43" t="s">
         <v>118</v>
       </c>
@@ -5202,21 +5782,26 @@
       <c r="D43" t="s">
         <v>542</v>
       </c>
-      <c r="E43" s="59"/>
+      <c r="E43" s="66" t="s">
+        <v>830</v>
+      </c>
       <c r="F43" s="66" t="s">
-        <v>785</v>
-      </c>
-      <c r="G43" s="66" t="s">
+        <v>783</v>
+      </c>
+      <c r="G43" t="s">
+        <v>886</v>
+      </c>
+      <c r="H43" s="66" t="s">
         <v>694</v>
       </c>
-      <c r="H43" s="66" t="s">
+      <c r="I43" s="66" t="s">
         <v>616</v>
       </c>
-      <c r="I43" s="56" t="s">
+      <c r="J43" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15">
+    <row r="44" spans="1:10" ht="15">
       <c r="A44" t="s">
         <v>432</v>
       </c>
@@ -5235,17 +5820,20 @@
       <c r="F44" s="56" t="s">
         <v>618</v>
       </c>
-      <c r="G44" s="56" t="s">
+      <c r="G44" t="s">
+        <v>887</v>
+      </c>
+      <c r="H44" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>619</v>
       </c>
-      <c r="I44" s="56" t="s">
+      <c r="J44" s="56" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15">
+    <row r="45" spans="1:10" ht="15">
       <c r="A45" t="s">
         <v>112</v>
       </c>
@@ -5258,20 +5846,26 @@
       <c r="D45" t="s">
         <v>542</v>
       </c>
+      <c r="E45" s="66" t="s">
+        <v>831</v>
+      </c>
       <c r="F45" s="66" t="s">
-        <v>786</v>
-      </c>
-      <c r="G45" s="66" t="s">
+        <v>784</v>
+      </c>
+      <c r="G45" t="s">
+        <v>888</v>
+      </c>
+      <c r="H45" s="66" t="s">
         <v>694</v>
       </c>
-      <c r="H45" s="66" t="s">
+      <c r="I45" s="66" t="s">
         <v>616</v>
       </c>
-      <c r="I45" s="56" t="s">
+      <c r="J45" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15">
+    <row r="46" spans="1:10" ht="15">
       <c r="A46" t="s">
         <v>438</v>
       </c>
@@ -5285,22 +5879,25 @@
         <v>623</v>
       </c>
       <c r="E46" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F46" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="G46" t="s">
+        <v>889</v>
+      </c>
+      <c r="H46" t="s">
         <v>694</v>
       </c>
-      <c r="H46" s="56" t="s">
-        <v>800</v>
-      </c>
       <c r="I46" s="56" t="s">
+        <v>798</v>
+      </c>
+      <c r="J46" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15">
+    <row r="47" spans="1:10" ht="15">
       <c r="A47" t="s">
         <v>420</v>
       </c>
@@ -5319,14 +5916,17 @@
       <c r="F47" t="s">
         <v>630</v>
       </c>
-      <c r="G47" s="56" t="s">
+      <c r="G47" t="s">
+        <v>890</v>
+      </c>
+      <c r="H47" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="I47" s="56" t="s">
+      <c r="J47" s="56" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15">
+    <row r="48" spans="1:10" ht="15">
       <c r="A48" s="26" t="s">
         <v>445</v>
       </c>
@@ -5339,14 +5939,14 @@
       <c r="D48" t="s">
         <v>557</v>
       </c>
-      <c r="H48" s="56" t="s">
+      <c r="I48" s="56" t="s">
         <v>626</v>
       </c>
-      <c r="I48" s="56" t="s">
+      <c r="J48" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15">
+    <row r="49" spans="1:10" ht="15">
       <c r="A49" t="s">
         <v>451</v>
       </c>
@@ -5359,20 +5959,26 @@
       <c r="D49" t="s">
         <v>499</v>
       </c>
+      <c r="E49" s="66" t="s">
+        <v>813</v>
+      </c>
       <c r="F49" s="67" t="s">
-        <v>809</v>
-      </c>
-      <c r="G49" s="65" t="s">
+        <v>807</v>
+      </c>
+      <c r="G49" t="s">
+        <v>891</v>
+      </c>
+      <c r="H49" s="65" t="s">
         <v>694</v>
       </c>
-      <c r="H49" s="67" t="s">
-        <v>808</v>
-      </c>
-      <c r="I49" s="56" t="s">
+      <c r="I49" s="67" t="s">
+        <v>806</v>
+      </c>
+      <c r="J49" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15">
+    <row r="50" spans="1:10" ht="15">
       <c r="A50" t="s">
         <v>114</v>
       </c>
@@ -5385,20 +5991,26 @@
       <c r="D50" t="s">
         <v>542</v>
       </c>
+      <c r="E50" s="66" t="s">
+        <v>832</v>
+      </c>
       <c r="F50" s="66" t="s">
-        <v>788</v>
-      </c>
-      <c r="G50" s="67" t="s">
+        <v>786</v>
+      </c>
+      <c r="G50" t="s">
+        <v>892</v>
+      </c>
+      <c r="H50" s="67" t="s">
         <v>694</v>
       </c>
-      <c r="H50" s="67" t="s">
+      <c r="I50" s="67" t="s">
         <v>543</v>
       </c>
-      <c r="I50" s="56" t="s">
+      <c r="J50" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15">
+    <row r="51" spans="1:10" ht="15">
       <c r="A51" t="s">
         <v>418</v>
       </c>
@@ -5411,14 +6023,14 @@
       <c r="D51" t="s">
         <v>506</v>
       </c>
-      <c r="H51" s="56" t="s">
+      <c r="I51" s="56" t="s">
         <v>632</v>
       </c>
-      <c r="I51" s="56" t="s">
+      <c r="J51" s="56" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15">
+    <row r="52" spans="1:10" ht="15">
       <c r="A52" t="s">
         <v>694</v>
       </c>
@@ -5431,20 +6043,26 @@
       <c r="D52" t="s">
         <v>557</v>
       </c>
+      <c r="E52" s="66" t="s">
+        <v>833</v>
+      </c>
       <c r="F52" s="71" t="s">
-        <v>791</v>
-      </c>
-      <c r="G52" s="71" t="s">
+        <v>789</v>
+      </c>
+      <c r="G52" t="s">
+        <v>893</v>
+      </c>
+      <c r="H52" s="71" t="s">
         <v>694</v>
       </c>
-      <c r="H52" s="26" t="s">
+      <c r="I52" s="26" t="s">
         <v>697</v>
       </c>
-      <c r="I52" s="56" t="s">
+      <c r="J52" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15">
+    <row r="53" spans="1:10" ht="15">
       <c r="A53" t="s">
         <v>694</v>
       </c>
@@ -5457,17 +6075,23 @@
       <c r="D53" t="s">
         <v>623</v>
       </c>
+      <c r="E53" s="66" t="s">
+        <v>834</v>
+      </c>
       <c r="F53" s="71" t="s">
-        <v>793</v>
-      </c>
-      <c r="G53" s="71" t="s">
+        <v>791</v>
+      </c>
+      <c r="G53" t="s">
+        <v>894</v>
+      </c>
+      <c r="H53" s="71" t="s">
         <v>694</v>
       </c>
-      <c r="I53" s="56" t="s">
+      <c r="J53" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15">
+    <row r="54" spans="1:10" ht="15">
       <c r="A54" t="s">
         <v>694</v>
       </c>
@@ -5480,17 +6104,23 @@
       <c r="D54" t="s">
         <v>623</v>
       </c>
+      <c r="E54" s="66" t="s">
+        <v>835</v>
+      </c>
       <c r="F54" s="71" t="s">
-        <v>794</v>
-      </c>
-      <c r="G54" s="71" t="s">
+        <v>792</v>
+      </c>
+      <c r="G54" t="s">
+        <v>895</v>
+      </c>
+      <c r="H54" s="71" t="s">
         <v>694</v>
       </c>
-      <c r="I54" s="56" t="s">
+      <c r="J54" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15">
+    <row r="55" spans="1:10" ht="15">
       <c r="A55" t="s">
         <v>694</v>
       </c>
@@ -5503,20 +6133,26 @@
       <c r="D55" t="s">
         <v>557</v>
       </c>
+      <c r="E55" s="66" t="s">
+        <v>835</v>
+      </c>
       <c r="F55" s="71" t="s">
-        <v>794</v>
-      </c>
-      <c r="G55" s="71" t="s">
+        <v>792</v>
+      </c>
+      <c r="G55" t="s">
+        <v>895</v>
+      </c>
+      <c r="H55" s="71" t="s">
         <v>694</v>
       </c>
-      <c r="H55" s="57" t="s">
+      <c r="I55" s="57" t="s">
         <v>700</v>
       </c>
-      <c r="I55" s="56" t="s">
+      <c r="J55" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15">
+    <row r="56" spans="1:10" ht="15">
       <c r="A56" t="s">
         <v>694</v>
       </c>
@@ -5529,18 +6165,24 @@
       <c r="D56" t="s">
         <v>557</v>
       </c>
+      <c r="E56" s="66" t="s">
+        <v>836</v>
+      </c>
       <c r="F56" s="71" t="s">
-        <v>792</v>
-      </c>
-      <c r="G56" s="71" t="s">
+        <v>790</v>
+      </c>
+      <c r="G56" t="s">
+        <v>896</v>
+      </c>
+      <c r="H56" s="71" t="s">
         <v>694</v>
       </c>
-      <c r="H56" s="65"/>
-      <c r="I56" s="56" t="s">
+      <c r="I56" s="65"/>
+      <c r="J56" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="15">
+    <row r="57" spans="1:10" ht="15">
       <c r="A57" t="s">
         <v>694</v>
       </c>
@@ -5553,20 +6195,26 @@
       <c r="D57" t="s">
         <v>557</v>
       </c>
+      <c r="E57" s="66" t="s">
+        <v>837</v>
+      </c>
       <c r="F57" s="71" t="s">
-        <v>807</v>
-      </c>
-      <c r="G57" s="71" t="s">
+        <v>805</v>
+      </c>
+      <c r="G57" t="s">
+        <v>897</v>
+      </c>
+      <c r="H57" s="71" t="s">
         <v>694</v>
       </c>
-      <c r="H57" s="65" t="s">
+      <c r="I57" s="65" t="s">
         <v>705</v>
       </c>
-      <c r="I57" s="56" t="s">
+      <c r="J57" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="15">
+    <row r="58" spans="1:10" ht="15">
       <c r="A58" t="s">
         <v>694</v>
       </c>
@@ -5579,17 +6227,23 @@
       <c r="D58" t="s">
         <v>623</v>
       </c>
+      <c r="E58" s="66" t="s">
+        <v>838</v>
+      </c>
       <c r="F58" s="71" t="s">
-        <v>795</v>
-      </c>
-      <c r="G58" s="71" t="s">
+        <v>793</v>
+      </c>
+      <c r="G58" t="s">
+        <v>898</v>
+      </c>
+      <c r="H58" s="71" t="s">
         <v>694</v>
       </c>
-      <c r="I58" s="56" t="s">
+      <c r="J58" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="59" spans="1:9" s="62" customFormat="1" ht="15">
+    <row r="59" spans="1:10" s="62" customFormat="1" ht="15">
       <c r="A59" t="s">
         <v>694</v>
       </c>
@@ -5602,19 +6256,24 @@
       <c r="D59" t="s">
         <v>623</v>
       </c>
-      <c r="E59"/>
+      <c r="E59" s="66" t="s">
+        <v>839</v>
+      </c>
       <c r="F59" s="71" t="s">
-        <v>796</v>
-      </c>
-      <c r="G59" s="71" t="s">
+        <v>794</v>
+      </c>
+      <c r="G59" t="s">
+        <v>899</v>
+      </c>
+      <c r="H59" s="71" t="s">
         <v>694</v>
       </c>
-      <c r="H59"/>
-      <c r="I59" s="56" t="s">
+      <c r="I59"/>
+      <c r="J59" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15">
+    <row r="60" spans="1:10" ht="15">
       <c r="A60" t="s">
         <v>434</v>
       </c>
@@ -5627,21 +6286,26 @@
       <c r="D60" t="s">
         <v>516</v>
       </c>
-      <c r="E60" s="59"/>
+      <c r="E60" s="66" t="s">
+        <v>840</v>
+      </c>
       <c r="F60" s="71" t="s">
         <v>760</v>
       </c>
-      <c r="G60" s="71" t="s">
+      <c r="G60" t="s">
+        <v>900</v>
+      </c>
+      <c r="H60" s="71" t="s">
         <v>694</v>
       </c>
-      <c r="H60" s="67" t="s">
+      <c r="I60" s="67" t="s">
         <v>569</v>
       </c>
-      <c r="I60" s="56" t="s">
+      <c r="J60" s="56" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="15">
+    <row r="61" spans="1:10" ht="15">
       <c r="A61" t="s">
         <v>464</v>
       </c>
@@ -5654,18 +6318,23 @@
       <c r="D61" t="s">
         <v>623</v>
       </c>
-      <c r="E61" s="56"/>
+      <c r="E61" s="66" t="s">
+        <v>841</v>
+      </c>
       <c r="F61" s="67" t="s">
-        <v>802</v>
-      </c>
-      <c r="G61" s="67" t="s">
+        <v>800</v>
+      </c>
+      <c r="G61" t="s">
+        <v>901</v>
+      </c>
+      <c r="H61" s="67" t="s">
         <v>694</v>
       </c>
-      <c r="I61" s="56" t="s">
+      <c r="J61" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="15">
+    <row r="62" spans="1:10" ht="15">
       <c r="A62" t="s">
         <v>465</v>
       </c>
@@ -5678,18 +6347,23 @@
       <c r="D62" t="s">
         <v>623</v>
       </c>
-      <c r="E62" s="56"/>
+      <c r="E62" s="66" t="s">
+        <v>842</v>
+      </c>
       <c r="F62" s="67" t="s">
-        <v>803</v>
-      </c>
-      <c r="G62" s="67" t="s">
+        <v>801</v>
+      </c>
+      <c r="G62" t="s">
+        <v>902</v>
+      </c>
+      <c r="H62" s="67" t="s">
         <v>694</v>
       </c>
-      <c r="I62" s="56" t="s">
+      <c r="J62" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15">
+    <row r="63" spans="1:10" ht="15">
       <c r="A63" t="s">
         <v>448</v>
       </c>
@@ -5702,21 +6376,26 @@
       <c r="D63" t="s">
         <v>499</v>
       </c>
-      <c r="E63" s="59"/>
+      <c r="E63" s="66" t="s">
+        <v>843</v>
+      </c>
       <c r="F63" s="66" t="s">
-        <v>789</v>
-      </c>
-      <c r="G63" s="66" t="s">
+        <v>787</v>
+      </c>
+      <c r="G63" t="s">
+        <v>903</v>
+      </c>
+      <c r="H63" s="66" t="s">
         <v>694</v>
       </c>
-      <c r="H63" s="67" t="s">
+      <c r="I63" s="67" t="s">
         <v>501</v>
       </c>
-      <c r="I63" s="56" t="s">
+      <c r="J63" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15">
+    <row r="64" spans="1:10" ht="15">
       <c r="A64" t="s">
         <v>440</v>
       </c>
@@ -5729,21 +6408,26 @@
       <c r="D64" t="s">
         <v>623</v>
       </c>
-      <c r="E64" s="59"/>
+      <c r="E64" s="66" t="s">
+        <v>844</v>
+      </c>
       <c r="F64" s="66" t="s">
         <v>761</v>
       </c>
-      <c r="G64" s="66" t="s">
+      <c r="G64" t="s">
+        <v>904</v>
+      </c>
+      <c r="H64" s="66" t="s">
         <v>694</v>
       </c>
-      <c r="H64" s="67" t="s">
+      <c r="I64" s="67" t="s">
         <v>569</v>
       </c>
-      <c r="I64" s="56" t="s">
+      <c r="J64" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="15">
+    <row r="65" spans="1:10" ht="15">
       <c r="A65" t="s">
         <v>439</v>
       </c>
@@ -5756,21 +6440,26 @@
       <c r="D65" t="s">
         <v>623</v>
       </c>
-      <c r="E65" s="59"/>
+      <c r="E65" s="66" t="s">
+        <v>845</v>
+      </c>
       <c r="F65" s="66" t="s">
-        <v>804</v>
-      </c>
-      <c r="G65" s="66" t="s">
+        <v>802</v>
+      </c>
+      <c r="G65" t="s">
+        <v>905</v>
+      </c>
+      <c r="H65" s="66" t="s">
         <v>694</v>
       </c>
-      <c r="H65" s="67" t="s">
+      <c r="I65" s="67" t="s">
         <v>543</v>
       </c>
-      <c r="I65" s="56" t="s">
+      <c r="J65" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="15">
+    <row r="66" spans="1:10" ht="15">
       <c r="A66" s="62" t="s">
         <v>53</v>
       </c>
@@ -5783,23 +6472,26 @@
       <c r="D66" s="62" t="s">
         <v>591</v>
       </c>
-      <c r="E66" s="73" t="s">
-        <v>762</v>
+      <c r="E66" t="s">
+        <v>848</v>
       </c>
       <c r="F66" s="62" t="s">
         <v>763</v>
       </c>
-      <c r="G66" s="67" t="s">
+      <c r="G66" t="s">
+        <v>762</v>
+      </c>
+      <c r="H66" s="67" t="s">
         <v>694</v>
       </c>
-      <c r="H66" s="76" t="s">
-        <v>798</v>
-      </c>
-      <c r="I66" s="73" t="s">
+      <c r="I66" s="76" t="s">
+        <v>796</v>
+      </c>
+      <c r="J66" s="73" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="15">
+    <row r="67" spans="1:10" ht="15">
       <c r="A67" t="s">
         <v>446</v>
       </c>
@@ -5812,21 +6504,26 @@
       <c r="D67" t="s">
         <v>516</v>
       </c>
-      <c r="E67" s="59"/>
+      <c r="E67" s="66" t="s">
+        <v>846</v>
+      </c>
       <c r="F67" s="66" t="s">
         <v>646</v>
       </c>
-      <c r="G67" s="66" t="s">
+      <c r="G67" t="s">
+        <v>906</v>
+      </c>
+      <c r="H67" s="66" t="s">
         <v>694</v>
       </c>
-      <c r="H67" s="67" t="s">
+      <c r="I67" s="67" t="s">
         <v>543</v>
       </c>
-      <c r="I67" s="56" t="s">
+      <c r="J67" s="56" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="15">
+    <row r="68" spans="1:10" ht="15">
       <c r="A68" t="s">
         <v>435</v>
       </c>
@@ -5839,21 +6536,26 @@
       <c r="D68" t="s">
         <v>623</v>
       </c>
-      <c r="E68" s="59"/>
-      <c r="F68" s="125" t="s">
-        <v>805</v>
-      </c>
-      <c r="G68" s="124" t="s">
+      <c r="E68" s="66" t="s">
+        <v>847</v>
+      </c>
+      <c r="F68" s="79" t="s">
+        <v>803</v>
+      </c>
+      <c r="G68" t="s">
+        <v>907</v>
+      </c>
+      <c r="H68" s="78" t="s">
         <v>694</v>
       </c>
-      <c r="H68" s="67" t="s">
+      <c r="I68" s="67" t="s">
         <v>543</v>
       </c>
-      <c r="I68" s="56" t="s">
+      <c r="J68" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="15">
+    <row r="69" spans="1:10" ht="15">
       <c r="A69" t="s">
         <v>428</v>
       </c>
@@ -5872,17 +6574,20 @@
       <c r="F69" s="63" t="s">
         <v>652</v>
       </c>
-      <c r="G69" s="63" t="s">
+      <c r="G69" t="s">
+        <v>908</v>
+      </c>
+      <c r="H69" s="63" t="s">
         <v>694</v>
       </c>
-      <c r="H69" t="s">
-        <v>797</v>
-      </c>
-      <c r="I69" s="56" t="s">
+      <c r="I69" t="s">
+        <v>795</v>
+      </c>
+      <c r="J69" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="15">
+    <row r="70" spans="1:10" ht="15">
       <c r="A70" t="s">
         <v>427</v>
       </c>
@@ -5901,17 +6606,20 @@
       <c r="F70" s="64" t="s">
         <v>656</v>
       </c>
-      <c r="G70" s="64" t="s">
+      <c r="G70" t="s">
+        <v>909</v>
+      </c>
+      <c r="H70" s="64" t="s">
         <v>694</v>
       </c>
-      <c r="H70" t="s">
+      <c r="I70" t="s">
         <v>533</v>
       </c>
-      <c r="I70" s="56" t="s">
+      <c r="J70" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="15">
+    <row r="71" spans="1:10" ht="15">
       <c r="A71" t="s">
         <v>399</v>
       </c>
@@ -5924,20 +6632,26 @@
       <c r="D71" t="s">
         <v>536</v>
       </c>
+      <c r="E71" s="126" t="s">
+        <v>813</v>
+      </c>
       <c r="F71" s="74" t="s">
         <v>657</v>
       </c>
-      <c r="G71" s="74" t="s">
+      <c r="G71" t="s">
+        <v>891</v>
+      </c>
+      <c r="H71" s="74" t="s">
         <v>694</v>
       </c>
-      <c r="H71" s="67" t="s">
+      <c r="I71" s="67" t="s">
         <v>658</v>
       </c>
-      <c r="I71" s="56" t="s">
+      <c r="J71" s="56" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="15">
+    <row r="72" spans="1:10" ht="15">
       <c r="A72" t="s">
         <v>694</v>
       </c>
@@ -5956,17 +6670,20 @@
       <c r="F72" t="s">
         <v>717</v>
       </c>
-      <c r="G72" s="56" t="s">
+      <c r="G72" t="s">
+        <v>910</v>
+      </c>
+      <c r="H72" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H72" t="s">
+      <c r="I72" t="s">
         <v>718</v>
       </c>
-      <c r="I72" s="56" t="s">
+      <c r="J72" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="15">
+    <row r="73" spans="1:10" ht="15">
       <c r="A73" t="s">
         <v>455</v>
       </c>
@@ -5979,20 +6696,26 @@
       <c r="D73" t="s">
         <v>494</v>
       </c>
+      <c r="E73" s="126" t="s">
+        <v>813</v>
+      </c>
       <c r="F73" s="74" t="s">
         <v>661</v>
       </c>
-      <c r="G73" s="74" t="s">
+      <c r="G73" t="s">
+        <v>891</v>
+      </c>
+      <c r="H73" s="74" t="s">
         <v>694</v>
       </c>
-      <c r="H73" s="67" t="s">
+      <c r="I73" s="67" t="s">
         <v>662</v>
       </c>
-      <c r="I73" s="56" t="s">
+      <c r="J73" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="15">
+    <row r="74" spans="1:10" ht="15">
       <c r="A74" t="s">
         <v>426</v>
       </c>
@@ -6011,17 +6734,20 @@
       <c r="F74" s="56" t="s">
         <v>666</v>
       </c>
-      <c r="G74" s="56" t="s">
+      <c r="G74" t="s">
+        <v>911</v>
+      </c>
+      <c r="H74" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H74" t="s">
+      <c r="I74" t="s">
         <v>533</v>
       </c>
-      <c r="I74" s="56" t="s">
+      <c r="J74" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="15">
+    <row r="75" spans="1:10" ht="15">
       <c r="A75" s="26" t="s">
         <v>16</v>
       </c>
@@ -6041,16 +6767,19 @@
         <v>757</v>
       </c>
       <c r="G75" t="s">
+        <v>570</v>
+      </c>
+      <c r="H75" t="s">
         <v>694</v>
       </c>
-      <c r="H75" t="s">
+      <c r="I75" t="s">
         <v>495</v>
       </c>
-      <c r="I75" s="56" t="s">
+      <c r="J75" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15">
+    <row r="76" spans="1:10" ht="15">
       <c r="A76" t="s">
         <v>85</v>
       </c>
@@ -6069,17 +6798,20 @@
       <c r="F76" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="G76" s="56" t="s">
+      <c r="G76" t="s">
+        <v>916</v>
+      </c>
+      <c r="H76" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H76" t="s">
-        <v>797</v>
-      </c>
-      <c r="I76" s="56" t="s">
+      <c r="I76" t="s">
+        <v>795</v>
+      </c>
+      <c r="J76" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="15">
+    <row r="77" spans="1:10" ht="15">
       <c r="A77" t="s">
         <v>398</v>
       </c>
@@ -6098,17 +6830,20 @@
       <c r="F77" s="56" t="s">
         <v>670</v>
       </c>
-      <c r="G77" s="56" t="s">
+      <c r="G77" t="s">
+        <v>912</v>
+      </c>
+      <c r="H77" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H77" t="s">
+      <c r="I77" t="s">
         <v>671</v>
       </c>
-      <c r="I77" s="56" t="s">
+      <c r="J77" s="56" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15">
+    <row r="78" spans="1:10" ht="15">
       <c r="A78" t="s">
         <v>413</v>
       </c>
@@ -6127,17 +6862,20 @@
       <c r="F78" s="56" t="s">
         <v>675</v>
       </c>
-      <c r="G78" s="56" t="s">
+      <c r="G78" t="s">
+        <v>913</v>
+      </c>
+      <c r="H78" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="H78" t="s">
+      <c r="I78" t="s">
         <v>676</v>
       </c>
-      <c r="I78" s="56" t="s">
+      <c r="J78" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="15">
+    <row r="79" spans="1:10" ht="15">
       <c r="A79" t="s">
         <v>412</v>
       </c>
@@ -6156,14 +6894,17 @@
       <c r="F79" s="56" t="s">
         <v>675</v>
       </c>
-      <c r="G79" s="56" t="s">
+      <c r="G79" t="s">
+        <v>913</v>
+      </c>
+      <c r="H79" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="I79" s="56" t="s">
+      <c r="J79" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="15">
+    <row r="80" spans="1:10" ht="15">
       <c r="A80" t="s">
         <v>409</v>
       </c>
@@ -6182,14 +6923,17 @@
       <c r="F80" s="56" t="s">
         <v>680</v>
       </c>
-      <c r="G80" s="56" t="s">
+      <c r="G80" t="s">
+        <v>914</v>
+      </c>
+      <c r="H80" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="I80" s="56" t="s">
+      <c r="J80" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="15">
+    <row r="81" spans="1:10" ht="15">
       <c r="A81" t="s">
         <v>424</v>
       </c>
@@ -6205,17 +6949,20 @@
       <c r="F81" s="73" t="s">
         <v>686</v>
       </c>
-      <c r="G81" s="123" t="s">
+      <c r="G81" t="s">
+        <v>915</v>
+      </c>
+      <c r="H81" s="77" t="s">
         <v>694</v>
       </c>
-      <c r="H81" t="s">
+      <c r="I81" t="s">
         <v>687</v>
       </c>
-      <c r="I81" s="56" t="s">
+      <c r="J81" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="15">
+    <row r="82" spans="1:10" ht="15">
       <c r="A82" t="s">
         <v>688</v>
       </c>
@@ -6228,20 +6975,26 @@
       <c r="D82" t="s">
         <v>544</v>
       </c>
+      <c r="E82" s="126" t="s">
+        <v>813</v>
+      </c>
       <c r="F82" s="66" t="s">
         <v>769</v>
       </c>
-      <c r="G82" s="66" t="s">
+      <c r="G82" t="s">
+        <v>891</v>
+      </c>
+      <c r="H82" s="66" t="s">
         <v>694</v>
       </c>
-      <c r="H82" s="67" t="s">
+      <c r="I82" s="67" t="s">
         <v>569</v>
       </c>
-      <c r="I82" s="56" t="s">
+      <c r="J82" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15">
+    <row r="83" spans="1:10" ht="15">
       <c r="A83" s="26" t="s">
         <v>437</v>
       </c>
@@ -6254,21 +7007,26 @@
       <c r="D83" s="26" t="s">
         <v>623</v>
       </c>
-      <c r="E83" s="26"/>
+      <c r="E83" s="126" t="s">
+        <v>813</v>
+      </c>
       <c r="F83" s="75" t="s">
-        <v>806</v>
-      </c>
-      <c r="G83" s="75" t="s">
+        <v>804</v>
+      </c>
+      <c r="G83" t="s">
+        <v>891</v>
+      </c>
+      <c r="H83" s="75" t="s">
         <v>694</v>
       </c>
-      <c r="H83" s="71" t="s">
+      <c r="I83" s="71" t="s">
         <v>569</v>
       </c>
-      <c r="I83" s="56" t="s">
+      <c r="J83" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="15">
+    <row r="84" spans="1:10" ht="15">
       <c r="A84" t="s">
         <v>116</v>
       </c>
@@ -6281,20 +7039,26 @@
       <c r="D84" t="s">
         <v>542</v>
       </c>
+      <c r="E84" s="126" t="s">
+        <v>813</v>
+      </c>
       <c r="F84" s="75" t="s">
-        <v>790</v>
-      </c>
-      <c r="G84" s="75" t="s">
+        <v>788</v>
+      </c>
+      <c r="G84" t="s">
+        <v>891</v>
+      </c>
+      <c r="H84" s="75" t="s">
         <v>694</v>
       </c>
-      <c r="H84" s="66" t="s">
+      <c r="I84" s="66" t="s">
         <v>764</v>
       </c>
-      <c r="I84" s="56" t="s">
+      <c r="J84" s="56" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:10">
       <c r="A87" s="65" t="s">
         <v>770</v>
       </c>
@@ -6302,7 +7066,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:10">
       <c r="A88" s="69" t="s">
         <v>772</v>
       </c>
@@ -6310,7 +7074,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:10">
       <c r="A89" s="67" t="s">
         <v>777</v>
       </c>
@@ -6318,7 +7082,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:10">
       <c r="A90" s="65" t="s">
         <v>775</v>
       </c>
@@ -7657,340 +8421,340 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="77" t="s">
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="101"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="101"/>
+      <c r="O1" s="101"/>
+      <c r="P1" s="101"/>
+      <c r="Q1" s="101"/>
+      <c r="R1" s="102"/>
+      <c r="S1" s="100" t="s">
         <v>417</v>
       </c>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
-      <c r="AC1" s="77"/>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="77"/>
-      <c r="AF1" s="77"/>
-      <c r="AG1" s="77"/>
-      <c r="AH1" s="77"/>
-      <c r="AI1" s="77"/>
-      <c r="AJ1" s="77"/>
-      <c r="AK1" s="77"/>
-      <c r="AL1" s="106" t="s">
+      <c r="T1" s="100"/>
+      <c r="U1" s="100"/>
+      <c r="V1" s="100"/>
+      <c r="W1" s="100"/>
+      <c r="X1" s="100"/>
+      <c r="Y1" s="100"/>
+      <c r="Z1" s="100"/>
+      <c r="AA1" s="100"/>
+      <c r="AB1" s="100"/>
+      <c r="AC1" s="100"/>
+      <c r="AD1" s="100"/>
+      <c r="AE1" s="100"/>
+      <c r="AF1" s="100"/>
+      <c r="AG1" s="100"/>
+      <c r="AH1" s="100"/>
+      <c r="AI1" s="100"/>
+      <c r="AJ1" s="100"/>
+      <c r="AK1" s="100"/>
+      <c r="AL1" s="86" t="s">
         <v>432</v>
       </c>
-      <c r="AM1" s="106"/>
-      <c r="AN1" s="106"/>
-      <c r="AO1" s="106"/>
-      <c r="AP1" s="106"/>
-      <c r="AQ1" s="106"/>
-      <c r="AR1" s="106"/>
-      <c r="AS1" s="106"/>
-      <c r="AT1" s="106"/>
-      <c r="AU1" s="106"/>
-      <c r="AV1" s="106"/>
-      <c r="AW1" s="106"/>
-      <c r="AX1" s="106"/>
-      <c r="AY1" s="106"/>
-      <c r="AZ1" s="106"/>
-      <c r="BA1" s="106"/>
-      <c r="BB1" s="106"/>
-      <c r="BC1" s="106"/>
-      <c r="BD1" s="106"/>
-      <c r="BE1" s="105" t="s">
+      <c r="AM1" s="86"/>
+      <c r="AN1" s="86"/>
+      <c r="AO1" s="86"/>
+      <c r="AP1" s="86"/>
+      <c r="AQ1" s="86"/>
+      <c r="AR1" s="86"/>
+      <c r="AS1" s="86"/>
+      <c r="AT1" s="86"/>
+      <c r="AU1" s="86"/>
+      <c r="AV1" s="86"/>
+      <c r="AW1" s="86"/>
+      <c r="AX1" s="86"/>
+      <c r="AY1" s="86"/>
+      <c r="AZ1" s="86"/>
+      <c r="BA1" s="86"/>
+      <c r="BB1" s="86"/>
+      <c r="BC1" s="86"/>
+      <c r="BD1" s="86"/>
+      <c r="BE1" s="85" t="s">
         <v>124</v>
       </c>
-      <c r="BF1" s="105"/>
-      <c r="BG1" s="105"/>
-      <c r="BH1" s="105"/>
-      <c r="BI1" s="103" t="s">
+      <c r="BF1" s="85"/>
+      <c r="BG1" s="85"/>
+      <c r="BH1" s="85"/>
+      <c r="BI1" s="82" t="s">
         <v>135</v>
       </c>
-      <c r="BJ1" s="103"/>
+      <c r="BJ1" s="82"/>
     </row>
     <row r="2" spans="1:62">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="103" t="s">
         <v>403</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="83" t="s">
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="105" t="s">
         <v>398</v>
       </c>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="83"/>
-      <c r="S2" s="90" t="s">
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="105"/>
+      <c r="S2" s="110" t="s">
         <v>418</v>
       </c>
-      <c r="T2" s="90"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="91" t="s">
+      <c r="T2" s="110"/>
+      <c r="U2" s="110"/>
+      <c r="V2" s="111" t="s">
         <v>419</v>
       </c>
-      <c r="W2" s="91"/>
-      <c r="X2" s="91"/>
-      <c r="Y2" s="91"/>
-      <c r="Z2" s="92" t="s">
+      <c r="W2" s="111"/>
+      <c r="X2" s="111"/>
+      <c r="Y2" s="111"/>
+      <c r="Z2" s="112" t="s">
         <v>420</v>
       </c>
-      <c r="AA2" s="92"/>
-      <c r="AB2" s="92"/>
-      <c r="AC2" s="92"/>
-      <c r="AD2" s="92"/>
-      <c r="AE2" s="92"/>
-      <c r="AF2" s="92"/>
-      <c r="AG2" s="92"/>
-      <c r="AH2" s="92"/>
-      <c r="AI2" s="92"/>
-      <c r="AJ2" s="92"/>
-      <c r="AK2" s="92"/>
-      <c r="AL2" s="108" t="s">
+      <c r="AA2" s="112"/>
+      <c r="AB2" s="112"/>
+      <c r="AC2" s="112"/>
+      <c r="AD2" s="112"/>
+      <c r="AE2" s="112"/>
+      <c r="AF2" s="112"/>
+      <c r="AG2" s="112"/>
+      <c r="AH2" s="112"/>
+      <c r="AI2" s="112"/>
+      <c r="AJ2" s="112"/>
+      <c r="AK2" s="112"/>
+      <c r="AL2" s="88" t="s">
         <v>434</v>
       </c>
-      <c r="AM2" s="108"/>
-      <c r="AN2" s="108"/>
-      <c r="AO2" s="108"/>
-      <c r="AP2" s="108"/>
-      <c r="AQ2" s="108"/>
-      <c r="AR2" s="108"/>
-      <c r="AS2" s="109" t="s">
+      <c r="AM2" s="88"/>
+      <c r="AN2" s="88"/>
+      <c r="AO2" s="88"/>
+      <c r="AP2" s="88"/>
+      <c r="AQ2" s="88"/>
+      <c r="AR2" s="88"/>
+      <c r="AS2" s="89" t="s">
         <v>433</v>
       </c>
-      <c r="AT2" s="109"/>
-      <c r="AU2" s="109"/>
-      <c r="AV2" s="109"/>
-      <c r="AW2" s="109"/>
-      <c r="AX2" s="107" t="s">
+      <c r="AT2" s="89"/>
+      <c r="AU2" s="89"/>
+      <c r="AV2" s="89"/>
+      <c r="AW2" s="89"/>
+      <c r="AX2" s="87" t="s">
         <v>446</v>
       </c>
-      <c r="AY2" s="107"/>
-      <c r="AZ2" s="107"/>
-      <c r="BA2" s="107"/>
-      <c r="BB2" s="107"/>
-      <c r="BC2" s="95" t="s">
+      <c r="AY2" s="87"/>
+      <c r="AZ2" s="87"/>
+      <c r="BA2" s="87"/>
+      <c r="BB2" s="87"/>
+      <c r="BC2" s="84" t="s">
         <v>447</v>
       </c>
-      <c r="BD2" s="82" t="s">
+      <c r="BD2" s="90" t="s">
         <v>122</v>
       </c>
-      <c r="BE2" s="104" t="s">
+      <c r="BE2" s="83" t="s">
         <v>449</v>
       </c>
-      <c r="BF2" s="104" t="s">
+      <c r="BF2" s="83" t="s">
         <v>448</v>
       </c>
-      <c r="BG2" s="104" t="s">
+      <c r="BG2" s="83" t="s">
         <v>450</v>
       </c>
-      <c r="BH2" s="104" t="s">
+      <c r="BH2" s="83" t="s">
         <v>451</v>
       </c>
-      <c r="BI2" s="104" t="s">
+      <c r="BI2" s="83" t="s">
         <v>452</v>
       </c>
-      <c r="BJ2" s="104" t="s">
+      <c r="BJ2" s="83" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:62" ht="15" customHeight="1">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="90" t="s">
         <v>455</v>
       </c>
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="91" t="s">
         <v>474</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="106" t="s">
         <v>409</v>
       </c>
-      <c r="D3" s="86" t="s">
+      <c r="D3" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="86" t="s">
+      <c r="E3" s="80" t="s">
         <v>400</v>
       </c>
-      <c r="F3" s="86" t="s">
+      <c r="F3" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="87" t="s">
+      <c r="G3" s="81" t="s">
         <v>479</v>
       </c>
-      <c r="H3" s="86" t="s">
+      <c r="H3" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="88" t="s">
+      <c r="I3" s="108" t="s">
         <v>399</v>
       </c>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="89" t="s">
+      <c r="J3" s="108"/>
+      <c r="K3" s="108"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="108"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="109" t="s">
         <v>405</v>
       </c>
-      <c r="P3" s="89"/>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="89"/>
-      <c r="S3" s="86" t="s">
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="80" t="s">
         <v>416</v>
       </c>
-      <c r="T3" s="86" t="s">
+      <c r="T3" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="U3" s="93" t="s">
+      <c r="U3" s="98" t="s">
         <v>477</v>
       </c>
-      <c r="V3" s="93" t="s">
+      <c r="V3" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="W3" s="86" t="s">
+      <c r="W3" s="80" t="s">
         <v>421</v>
       </c>
-      <c r="X3" s="94" t="s">
+      <c r="X3" s="99" t="s">
         <v>424</v>
       </c>
-      <c r="Y3" s="87" t="s">
+      <c r="Y3" s="81" t="s">
         <v>478</v>
       </c>
-      <c r="Z3" s="86" t="s">
+      <c r="Z3" s="80" t="s">
         <v>426</v>
       </c>
-      <c r="AA3" s="87" t="s">
+      <c r="AA3" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="AB3" s="86" t="s">
+      <c r="AB3" s="80" t="s">
         <v>427</v>
       </c>
-      <c r="AC3" s="86" t="s">
+      <c r="AC3" s="80" t="s">
         <v>429</v>
       </c>
-      <c r="AD3" s="87" t="s">
+      <c r="AD3" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="AE3" s="87" t="s">
+      <c r="AE3" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="AF3" s="87" t="s">
+      <c r="AF3" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="AG3" s="86" t="s">
+      <c r="AG3" s="80" t="s">
         <v>428</v>
       </c>
-      <c r="AH3" s="86" t="s">
+      <c r="AH3" s="80" t="s">
         <v>430</v>
       </c>
-      <c r="AI3" s="87" t="s">
+      <c r="AI3" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="AJ3" s="101" t="s">
+      <c r="AJ3" s="93" t="s">
         <v>468</v>
       </c>
-      <c r="AK3" s="86" t="s">
+      <c r="AK3" s="80" t="s">
         <v>431</v>
       </c>
-      <c r="AL3" s="96" t="s">
+      <c r="AL3" s="97" t="s">
         <v>435</v>
       </c>
-      <c r="AM3" s="96" t="s">
+      <c r="AM3" s="97" t="s">
         <v>437</v>
       </c>
-      <c r="AN3" s="96" t="s">
+      <c r="AN3" s="97" t="s">
         <v>438</v>
       </c>
-      <c r="AO3" s="97" t="s">
+      <c r="AO3" s="95" t="s">
         <v>464</v>
       </c>
-      <c r="AP3" s="96" t="s">
+      <c r="AP3" s="97" t="s">
         <v>439</v>
       </c>
-      <c r="AQ3" s="97" t="s">
+      <c r="AQ3" s="95" t="s">
         <v>465</v>
       </c>
-      <c r="AR3" s="96" t="s">
+      <c r="AR3" s="97" t="s">
         <v>440</v>
       </c>
-      <c r="AS3" s="82" t="s">
+      <c r="AS3" s="90" t="s">
         <v>99</v>
       </c>
-      <c r="AT3" s="95" t="s">
+      <c r="AT3" s="84" t="s">
         <v>441</v>
       </c>
-      <c r="AU3" s="95" t="s">
+      <c r="AU3" s="84" t="s">
         <v>442</v>
       </c>
-      <c r="AV3" s="95" t="s">
+      <c r="AV3" s="84" t="s">
         <v>443</v>
       </c>
-      <c r="AW3" s="95" t="s">
+      <c r="AW3" s="84" t="s">
         <v>445</v>
       </c>
-      <c r="AX3" s="95" t="s">
+      <c r="AX3" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="AY3" s="95" t="s">
+      <c r="AY3" s="84" t="s">
         <v>112</v>
       </c>
-      <c r="AZ3" s="95" t="s">
+      <c r="AZ3" s="84" t="s">
         <v>114</v>
       </c>
-      <c r="BA3" s="95" t="s">
+      <c r="BA3" s="84" t="s">
         <v>116</v>
       </c>
-      <c r="BB3" s="95" t="s">
+      <c r="BB3" s="84" t="s">
         <v>118</v>
       </c>
-      <c r="BC3" s="95"/>
-      <c r="BD3" s="82"/>
-      <c r="BE3" s="104"/>
-      <c r="BF3" s="104"/>
-      <c r="BG3" s="104"/>
-      <c r="BH3" s="104"/>
-      <c r="BI3" s="104"/>
-      <c r="BJ3" s="104"/>
+      <c r="BC3" s="84"/>
+      <c r="BD3" s="90"/>
+      <c r="BE3" s="83"/>
+      <c r="BF3" s="83"/>
+      <c r="BG3" s="83"/>
+      <c r="BH3" s="83"/>
+      <c r="BI3" s="83"/>
+      <c r="BJ3" s="83"/>
     </row>
     <row r="4" spans="1:62">
-      <c r="A4" s="82"/>
-      <c r="B4" s="100"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
+      <c r="A4" s="90"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
       <c r="I4" s="20" t="s">
         <v>401</v>
       </c>
@@ -8021,50 +8785,50 @@
       <c r="R4" s="20" t="s">
         <v>415</v>
       </c>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="93"/>
-      <c r="V4" s="93"/>
-      <c r="W4" s="87"/>
-      <c r="X4" s="93"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="86"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="86"/>
-      <c r="AC4" s="86"/>
-      <c r="AD4" s="87"/>
-      <c r="AE4" s="87"/>
-      <c r="AF4" s="87"/>
-      <c r="AG4" s="86"/>
-      <c r="AH4" s="87"/>
-      <c r="AI4" s="87"/>
-      <c r="AJ4" s="102"/>
-      <c r="AK4" s="86"/>
-      <c r="AL4" s="96"/>
-      <c r="AM4" s="96"/>
-      <c r="AN4" s="96"/>
-      <c r="AO4" s="98"/>
-      <c r="AP4" s="96"/>
-      <c r="AQ4" s="98"/>
-      <c r="AR4" s="96"/>
-      <c r="AS4" s="82"/>
-      <c r="AT4" s="95"/>
-      <c r="AU4" s="95"/>
-      <c r="AV4" s="95"/>
-      <c r="AW4" s="95"/>
-      <c r="AX4" s="95"/>
-      <c r="AY4" s="95"/>
-      <c r="AZ4" s="95"/>
-      <c r="BA4" s="95"/>
-      <c r="BB4" s="95"/>
-      <c r="BC4" s="95"/>
-      <c r="BD4" s="82"/>
-      <c r="BE4" s="104"/>
-      <c r="BF4" s="104"/>
-      <c r="BG4" s="104"/>
-      <c r="BH4" s="104"/>
-      <c r="BI4" s="104"/>
-      <c r="BJ4" s="104"/>
+      <c r="S4" s="80"/>
+      <c r="T4" s="80"/>
+      <c r="U4" s="98"/>
+      <c r="V4" s="98"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="98"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="80"/>
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="80"/>
+      <c r="AC4" s="80"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="81"/>
+      <c r="AG4" s="80"/>
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="94"/>
+      <c r="AK4" s="80"/>
+      <c r="AL4" s="97"/>
+      <c r="AM4" s="97"/>
+      <c r="AN4" s="97"/>
+      <c r="AO4" s="96"/>
+      <c r="AP4" s="97"/>
+      <c r="AQ4" s="96"/>
+      <c r="AR4" s="97"/>
+      <c r="AS4" s="90"/>
+      <c r="AT4" s="84"/>
+      <c r="AU4" s="84"/>
+      <c r="AV4" s="84"/>
+      <c r="AW4" s="84"/>
+      <c r="AX4" s="84"/>
+      <c r="AY4" s="84"/>
+      <c r="AZ4" s="84"/>
+      <c r="BA4" s="84"/>
+      <c r="BB4" s="84"/>
+      <c r="BC4" s="84"/>
+      <c r="BD4" s="90"/>
+      <c r="BE4" s="83"/>
+      <c r="BF4" s="83"/>
+      <c r="BG4" s="83"/>
+      <c r="BH4" s="83"/>
+      <c r="BI4" s="83"/>
+      <c r="BJ4" s="83"/>
     </row>
     <row r="5" spans="1:62">
       <c r="A5" s="21"/>
@@ -9561,6 +10325,57 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="67">
+    <mergeCell ref="S1:AK1"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="G2:R2"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="Z2:AK2"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="BC2:BC4"/>
+    <mergeCell ref="AL3:AL4"/>
+    <mergeCell ref="AM3:AM4"/>
+    <mergeCell ref="AN3:AN4"/>
+    <mergeCell ref="AP3:AP4"/>
+    <mergeCell ref="AR3:AR4"/>
+    <mergeCell ref="AS3:AS4"/>
+    <mergeCell ref="AW3:AW4"/>
+    <mergeCell ref="AX3:AX4"/>
+    <mergeCell ref="AY3:AY4"/>
+    <mergeCell ref="AZ3:AZ4"/>
+    <mergeCell ref="AO3:AO4"/>
+    <mergeCell ref="AV3:AV4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AJ3:AJ4"/>
+    <mergeCell ref="AT3:AT4"/>
+    <mergeCell ref="AU3:AU4"/>
+    <mergeCell ref="AQ3:AQ4"/>
+    <mergeCell ref="AG3:AG4"/>
+    <mergeCell ref="AH3:AH4"/>
+    <mergeCell ref="AI3:AI4"/>
+    <mergeCell ref="AK3:AK4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="BI1:BJ1"/>
     <mergeCell ref="BI2:BI4"/>
@@ -9577,57 +10392,6 @@
     <mergeCell ref="AL2:AR2"/>
     <mergeCell ref="AS2:AW2"/>
     <mergeCell ref="BD2:BD4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AJ3:AJ4"/>
-    <mergeCell ref="AT3:AT4"/>
-    <mergeCell ref="AU3:AU4"/>
-    <mergeCell ref="AQ3:AQ4"/>
-    <mergeCell ref="AG3:AG4"/>
-    <mergeCell ref="AH3:AH4"/>
-    <mergeCell ref="AI3:AI4"/>
-    <mergeCell ref="AK3:AK4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="BC2:BC4"/>
-    <mergeCell ref="AL3:AL4"/>
-    <mergeCell ref="AM3:AM4"/>
-    <mergeCell ref="AN3:AN4"/>
-    <mergeCell ref="AP3:AP4"/>
-    <mergeCell ref="AR3:AR4"/>
-    <mergeCell ref="AS3:AS4"/>
-    <mergeCell ref="AW3:AW4"/>
-    <mergeCell ref="AX3:AX4"/>
-    <mergeCell ref="AY3:AY4"/>
-    <mergeCell ref="AZ3:AZ4"/>
-    <mergeCell ref="AO3:AO4"/>
-    <mergeCell ref="AV3:AV4"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="S1:AK1"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="G2:R2"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="Z2:AK2"/>
-    <mergeCell ref="S3:S4"/>
   </mergeCells>
   <dataValidations xWindow="597" yWindow="252" count="91">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Gametocytes present" sqref="AS3"/>
@@ -11331,12 +12095,12 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="111"/>
-      <c r="C2" s="111"/>
-      <c r="D2" s="112"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="115"/>
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5">
@@ -11551,12 +12315,12 @@
       <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="113" t="s">
+      <c r="A18" s="116" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="114"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="115"/>
+      <c r="B18" s="117"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="118"/>
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" ht="28">
@@ -11841,12 +12605,12 @@
       <c r="E37" s="13"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="116" t="s">
+      <c r="A38" s="119" t="s">
         <v>89</v>
       </c>
-      <c r="B38" s="117"/>
-      <c r="C38" s="117"/>
-      <c r="D38" s="118"/>
+      <c r="B38" s="120"/>
+      <c r="C38" s="120"/>
+      <c r="D38" s="121"/>
       <c r="E38" s="13"/>
     </row>
     <row r="39" spans="1:5" ht="42">
@@ -12117,13 +12881,13 @@
       <c r="E57" s="13"/>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="119" t="s">
+      <c r="A58" s="122" t="s">
         <v>124</v>
       </c>
-      <c r="B58" s="120"/>
-      <c r="C58" s="120"/>
-      <c r="D58" s="120"/>
-      <c r="E58" s="120"/>
+      <c r="B58" s="123"/>
+      <c r="C58" s="123"/>
+      <c r="D58" s="123"/>
+      <c r="E58" s="123"/>
     </row>
     <row r="59" spans="1:5" ht="28">
       <c r="A59" s="15" t="s">
@@ -12186,12 +12950,12 @@
       <c r="E62" s="15"/>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="121" t="s">
+      <c r="A63" s="124" t="s">
         <v>135</v>
       </c>
-      <c r="B63" s="121"/>
-      <c r="C63" s="121"/>
-      <c r="D63" s="122"/>
+      <c r="B63" s="124"/>
+      <c r="C63" s="124"/>
+      <c r="D63" s="125"/>
       <c r="E63" s="15"/>
     </row>
     <row r="64" spans="1:5" ht="70">

</xml_diff>

<commit_message>
correct incorrect mapped ontology term IDs
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@82969 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ICEMR/ICEMR protein array/ICEMR submission form v3 ontology mapping.xlsx
+++ b/Load/src/ontology/ICEMR/ICEMR protein array/ICEMR submission form v3 ontology mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26423"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="2920" windowWidth="30780" windowHeight="14800"/>
+    <workbookView xWindow="2100" yWindow="2000" windowWidth="30780" windowHeight="14800"/>
   </bookViews>
   <sheets>
     <sheet name="terms" sheetId="5" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1737" uniqueCount="917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="927">
   <si>
     <t>uniqueid</t>
   </si>
@@ -2842,6 +2842,36 @@
   </si>
   <si>
     <t>SNOMEDCT_27942005</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000545</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000542</t>
+  </si>
+  <si>
+    <t>EUPATH_0000542</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000543</t>
+  </si>
+  <si>
+    <t>EUPATH_0000543</t>
+  </si>
+  <si>
+    <t>EUPATH_0000545</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000544</t>
+  </si>
+  <si>
+    <t>EUPATH_0000544</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000524</t>
+  </si>
+  <si>
+    <t>EUPATH_0000524</t>
   </si>
 </sst>
 </file>
@@ -3355,7 +3385,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="241">
+  <cellStyleXfs count="245">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3597,8 +3627,12 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3751,19 +3785,89 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3779,75 +3883,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3889,9 +3924,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="241">
+  <cellStyles count="245">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4018,6 +4053,8 @@
     <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
@@ -4131,6 +4168,8 @@
     <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -4442,24 +4481,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E57" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A7" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="41.83203125" customWidth="1"/>
-    <col min="5" max="5" width="50.6640625" customWidth="1"/>
+    <col min="2" max="2" width="44.5" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" customWidth="1"/>
+    <col min="4" max="4" width="37" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" style="127" customWidth="1"/>
     <col min="6" max="6" width="42.33203125" customWidth="1"/>
     <col min="7" max="7" width="19.5" customWidth="1"/>
     <col min="8" max="8" width="5.6640625" customWidth="1"/>
     <col min="9" max="9" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15">
+    <row r="1" spans="1:10">
       <c r="A1" s="54" t="s">
         <v>480</v>
       </c>
@@ -4491,7 +4530,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>430</v>
       </c>
@@ -4504,7 +4543,7 @@
       <c r="D2" t="s">
         <v>490</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="127" t="s">
         <v>491</v>
       </c>
       <c r="F2" t="s">
@@ -4523,7 +4562,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>400</v>
       </c>
@@ -4536,7 +4575,7 @@
       <c r="D3" t="s">
         <v>494</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="127" t="s">
         <v>752</v>
       </c>
       <c r="F3" t="s">
@@ -4555,7 +4594,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>429</v>
       </c>
@@ -4568,7 +4607,7 @@
       <c r="D4" t="s">
         <v>490</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="127" t="s">
         <v>497</v>
       </c>
       <c r="F4" t="s">
@@ -4587,7 +4626,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -4619,7 +4658,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -4632,7 +4671,7 @@
       <c r="D6" t="s">
         <v>490</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="127" t="s">
         <v>504</v>
       </c>
       <c r="F6" t="s">
@@ -4651,7 +4690,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>417</v>
       </c>
@@ -4664,7 +4703,7 @@
       <c r="D7" t="s">
         <v>500</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="127" t="s">
         <v>507</v>
       </c>
       <c r="F7" t="s">
@@ -4683,7 +4722,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>414</v>
       </c>
@@ -4715,7 +4754,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>468</v>
       </c>
@@ -4747,7 +4786,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -4779,7 +4818,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -4811,7 +4850,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>401</v>
       </c>
@@ -4824,7 +4863,7 @@
       <c r="D12" t="s">
         <v>524</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="127" t="s">
         <v>766</v>
       </c>
       <c r="F12" s="56" t="s">
@@ -4843,7 +4882,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>452</v>
       </c>
@@ -4875,7 +4914,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -4907,7 +4946,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -4920,7 +4959,7 @@
       <c r="D15" t="s">
         <v>536</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="127" t="s">
         <v>767</v>
       </c>
       <c r="F15" t="s">
@@ -4939,7 +4978,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>431</v>
       </c>
@@ -4971,7 +5010,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -5003,7 +5042,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15">
+    <row r="18" spans="1:10">
       <c r="A18" s="26" t="s">
         <v>419</v>
       </c>
@@ -5035,7 +5074,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>421</v>
       </c>
@@ -5065,7 +5104,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>415</v>
       </c>
@@ -5097,7 +5136,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>453</v>
       </c>
@@ -5129,7 +5168,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15">
+    <row r="22" spans="1:10">
       <c r="A22" s="26" t="s">
         <v>433</v>
       </c>
@@ -5161,7 +5200,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>441</v>
       </c>
@@ -5193,7 +5232,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>442</v>
       </c>
@@ -5225,7 +5264,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -5257,7 +5296,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>443</v>
       </c>
@@ -5289,7 +5328,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -5309,7 +5348,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>403</v>
       </c>
@@ -5322,7 +5361,7 @@
       <c r="D28" t="s">
         <v>572</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="127" t="s">
         <v>574</v>
       </c>
       <c r="F28" t="s">
@@ -5341,7 +5380,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15">
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>411</v>
       </c>
@@ -5373,7 +5412,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>404</v>
       </c>
@@ -5405,7 +5444,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>410</v>
       </c>
@@ -5437,7 +5476,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>408</v>
       </c>
@@ -5461,7 +5500,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>416</v>
       </c>
@@ -5493,7 +5532,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>447</v>
       </c>
@@ -5525,7 +5564,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15">
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -5538,7 +5577,7 @@
       <c r="D35" t="s">
         <v>591</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="127" t="s">
         <v>599</v>
       </c>
       <c r="F35" t="s">
@@ -5557,7 +5596,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15">
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>449</v>
       </c>
@@ -5589,7 +5628,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -5621,7 +5660,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15">
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>450</v>
       </c>
@@ -5653,7 +5692,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>405</v>
       </c>
@@ -5673,7 +5712,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15">
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>135</v>
       </c>
@@ -5705,7 +5744,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15">
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>474</v>
       </c>
@@ -5737,7 +5776,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15">
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>73</v>
       </c>
@@ -5769,7 +5808,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15">
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>118</v>
       </c>
@@ -5801,7 +5840,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15">
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>432</v>
       </c>
@@ -5833,7 +5872,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15">
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>112</v>
       </c>
@@ -5865,7 +5904,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15">
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>438</v>
       </c>
@@ -5878,7 +5917,7 @@
       <c r="D46" t="s">
         <v>623</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="127" t="s">
         <v>797</v>
       </c>
       <c r="F46" t="s">
@@ -5897,7 +5936,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15">
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>420</v>
       </c>
@@ -5910,7 +5949,7 @@
       <c r="D47" t="s">
         <v>506</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="127" t="s">
         <v>629</v>
       </c>
       <c r="F47" t="s">
@@ -5926,7 +5965,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15">
+    <row r="48" spans="1:10">
       <c r="A48" s="26" t="s">
         <v>445</v>
       </c>
@@ -5946,7 +5985,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15">
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>451</v>
       </c>
@@ -5978,7 +6017,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15">
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>114</v>
       </c>
@@ -6010,7 +6049,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15">
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>418</v>
       </c>
@@ -6030,10 +6069,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15">
-      <c r="A52" t="s">
-        <v>694</v>
-      </c>
+    <row r="52" spans="1:10">
       <c r="B52" t="s">
         <v>695</v>
       </c>
@@ -6062,10 +6098,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15">
-      <c r="A53" t="s">
-        <v>694</v>
-      </c>
+    <row r="53" spans="1:10">
       <c r="B53" t="s">
         <v>706</v>
       </c>
@@ -6091,10 +6124,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15">
-      <c r="A54" t="s">
-        <v>694</v>
-      </c>
+    <row r="54" spans="1:10">
       <c r="B54" t="s">
         <v>708</v>
       </c>
@@ -6120,10 +6150,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15">
-      <c r="A55" t="s">
-        <v>694</v>
-      </c>
+    <row r="55" spans="1:10">
       <c r="B55" t="s">
         <v>698</v>
       </c>
@@ -6152,10 +6179,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15">
-      <c r="A56" t="s">
-        <v>694</v>
-      </c>
+    <row r="56" spans="1:10">
       <c r="B56" t="s">
         <v>701</v>
       </c>
@@ -6182,10 +6206,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15">
-      <c r="A57" t="s">
-        <v>694</v>
-      </c>
+    <row r="57" spans="1:10">
       <c r="B57" t="s">
         <v>703</v>
       </c>
@@ -6214,10 +6235,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15">
-      <c r="A58" t="s">
-        <v>694</v>
-      </c>
+    <row r="58" spans="1:10">
       <c r="B58" t="s">
         <v>710</v>
       </c>
@@ -6243,10 +6261,8 @@
         <v>492</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="62" customFormat="1" ht="15">
-      <c r="A59" t="s">
-        <v>694</v>
-      </c>
+    <row r="59" spans="1:10" s="62" customFormat="1">
+      <c r="A59"/>
       <c r="B59" t="s">
         <v>712</v>
       </c>
@@ -6273,7 +6289,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15">
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
         <v>434</v>
       </c>
@@ -6305,7 +6321,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15">
+    <row r="61" spans="1:10">
       <c r="A61" t="s">
         <v>464</v>
       </c>
@@ -6334,7 +6350,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="15">
+    <row r="62" spans="1:10">
       <c r="A62" t="s">
         <v>465</v>
       </c>
@@ -6363,7 +6379,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="15">
+    <row r="63" spans="1:10">
       <c r="A63" t="s">
         <v>448</v>
       </c>
@@ -6395,7 +6411,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15">
+    <row r="64" spans="1:10">
       <c r="A64" t="s">
         <v>440</v>
       </c>
@@ -6427,7 +6443,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="15">
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
         <v>439</v>
       </c>
@@ -6459,7 +6475,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="15">
+    <row r="66" spans="1:10">
       <c r="A66" s="62" t="s">
         <v>53</v>
       </c>
@@ -6472,7 +6488,7 @@
       <c r="D66" s="62" t="s">
         <v>591</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="127" t="s">
         <v>848</v>
       </c>
       <c r="F66" s="62" t="s">
@@ -6491,7 +6507,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15">
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
         <v>446</v>
       </c>
@@ -6523,7 +6539,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="15">
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
         <v>435</v>
       </c>
@@ -6555,7 +6571,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="15">
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
         <v>428</v>
       </c>
@@ -6587,7 +6603,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="15">
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
         <v>427</v>
       </c>
@@ -6619,7 +6635,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="15">
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
         <v>399</v>
       </c>
@@ -6632,14 +6648,14 @@
       <c r="D71" t="s">
         <v>536</v>
       </c>
-      <c r="E71" s="126" t="s">
-        <v>813</v>
+      <c r="E71" s="127" t="s">
+        <v>918</v>
       </c>
       <c r="F71" s="74" t="s">
         <v>657</v>
       </c>
       <c r="G71" t="s">
-        <v>891</v>
+        <v>919</v>
       </c>
       <c r="H71" s="74" t="s">
         <v>694</v>
@@ -6651,9 +6667,9 @@
         <v>502</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="15">
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>694</v>
+        <v>479</v>
       </c>
       <c r="B72" t="s">
         <v>714</v>
@@ -6664,7 +6680,7 @@
       <c r="D72" t="s">
         <v>536</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="127" t="s">
         <v>716</v>
       </c>
       <c r="F72" t="s">
@@ -6683,7 +6699,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15">
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
         <v>455</v>
       </c>
@@ -6696,14 +6712,14 @@
       <c r="D73" t="s">
         <v>494</v>
       </c>
-      <c r="E73" s="126" t="s">
-        <v>813</v>
+      <c r="E73" s="80" t="s">
+        <v>920</v>
       </c>
       <c r="F73" s="74" t="s">
         <v>661</v>
       </c>
       <c r="G73" t="s">
-        <v>891</v>
+        <v>921</v>
       </c>
       <c r="H73" s="74" t="s">
         <v>694</v>
@@ -6715,7 +6731,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15">
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
         <v>426</v>
       </c>
@@ -6747,7 +6763,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="15">
+    <row r="75" spans="1:10">
       <c r="A75" s="26" t="s">
         <v>16</v>
       </c>
@@ -6760,7 +6776,7 @@
       <c r="D75" t="s">
         <v>494</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="127" t="s">
         <v>758</v>
       </c>
       <c r="F75" t="s">
@@ -6779,7 +6795,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="15">
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
         <v>85</v>
       </c>
@@ -6811,7 +6827,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="15">
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
         <v>398</v>
       </c>
@@ -6843,7 +6859,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15">
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
         <v>413</v>
       </c>
@@ -6875,7 +6891,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="15">
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
         <v>412</v>
       </c>
@@ -6904,7 +6920,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="15">
+    <row r="80" spans="1:10">
       <c r="A80" t="s">
         <v>409</v>
       </c>
@@ -6933,7 +6949,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="15">
+    <row r="81" spans="1:10">
       <c r="A81" t="s">
         <v>424</v>
       </c>
@@ -6943,7 +6959,7 @@
       <c r="C81" t="s">
         <v>684</v>
       </c>
-      <c r="E81" s="73" t="s">
+      <c r="E81" s="127" t="s">
         <v>685</v>
       </c>
       <c r="F81" s="73" t="s">
@@ -6962,7 +6978,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="15">
+    <row r="82" spans="1:10">
       <c r="A82" t="s">
         <v>688</v>
       </c>
@@ -6975,14 +6991,14 @@
       <c r="D82" t="s">
         <v>544</v>
       </c>
-      <c r="E82" s="126" t="s">
-        <v>813</v>
+      <c r="E82" s="80" t="s">
+        <v>923</v>
       </c>
       <c r="F82" s="66" t="s">
         <v>769</v>
       </c>
       <c r="G82" t="s">
-        <v>891</v>
+        <v>924</v>
       </c>
       <c r="H82" s="66" t="s">
         <v>694</v>
@@ -6994,7 +7010,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="15">
+    <row r="83" spans="1:10">
       <c r="A83" s="26" t="s">
         <v>437</v>
       </c>
@@ -7007,14 +7023,14 @@
       <c r="D83" s="26" t="s">
         <v>623</v>
       </c>
-      <c r="E83" s="126" t="s">
-        <v>813</v>
+      <c r="E83" s="127" t="s">
+        <v>917</v>
       </c>
       <c r="F83" s="75" t="s">
         <v>804</v>
       </c>
       <c r="G83" t="s">
-        <v>891</v>
+        <v>922</v>
       </c>
       <c r="H83" s="75" t="s">
         <v>694</v>
@@ -7026,7 +7042,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="15">
+    <row r="84" spans="1:10">
       <c r="A84" t="s">
         <v>116</v>
       </c>
@@ -7039,14 +7055,14 @@
       <c r="D84" t="s">
         <v>542</v>
       </c>
-      <c r="E84" s="126" t="s">
-        <v>813</v>
+      <c r="E84" s="80" t="s">
+        <v>925</v>
       </c>
       <c r="F84" s="75" t="s">
         <v>788</v>
       </c>
       <c r="G84" t="s">
-        <v>891</v>
+        <v>926</v>
       </c>
       <c r="H84" s="75" t="s">
         <v>694</v>
@@ -7091,9 +7107,6 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:I84">
-    <sortCondition ref="C2:C84"/>
-  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -8365,8 +8378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ227"/>
   <sheetViews>
-    <sheetView topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AL3" sqref="AL3:AL4"/>
+    <sheetView topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AK23" sqref="AK23:AU23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8421,340 +8434,340 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="101"/>
-      <c r="P1" s="101"/>
-      <c r="Q1" s="101"/>
-      <c r="R1" s="102"/>
-      <c r="S1" s="100" t="s">
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="81" t="s">
         <v>417</v>
       </c>
-      <c r="T1" s="100"/>
-      <c r="U1" s="100"/>
-      <c r="V1" s="100"/>
-      <c r="W1" s="100"/>
-      <c r="X1" s="100"/>
-      <c r="Y1" s="100"/>
-      <c r="Z1" s="100"/>
-      <c r="AA1" s="100"/>
-      <c r="AB1" s="100"/>
-      <c r="AC1" s="100"/>
-      <c r="AD1" s="100"/>
-      <c r="AE1" s="100"/>
-      <c r="AF1" s="100"/>
-      <c r="AG1" s="100"/>
-      <c r="AH1" s="100"/>
-      <c r="AI1" s="100"/>
-      <c r="AJ1" s="100"/>
-      <c r="AK1" s="100"/>
-      <c r="AL1" s="86" t="s">
+      <c r="T1" s="81"/>
+      <c r="U1" s="81"/>
+      <c r="V1" s="81"/>
+      <c r="W1" s="81"/>
+      <c r="X1" s="81"/>
+      <c r="Y1" s="81"/>
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="81"/>
+      <c r="AB1" s="81"/>
+      <c r="AC1" s="81"/>
+      <c r="AD1" s="81"/>
+      <c r="AE1" s="81"/>
+      <c r="AF1" s="81"/>
+      <c r="AG1" s="81"/>
+      <c r="AH1" s="81"/>
+      <c r="AI1" s="81"/>
+      <c r="AJ1" s="81"/>
+      <c r="AK1" s="81"/>
+      <c r="AL1" s="110" t="s">
         <v>432</v>
       </c>
-      <c r="AM1" s="86"/>
-      <c r="AN1" s="86"/>
-      <c r="AO1" s="86"/>
-      <c r="AP1" s="86"/>
-      <c r="AQ1" s="86"/>
-      <c r="AR1" s="86"/>
-      <c r="AS1" s="86"/>
-      <c r="AT1" s="86"/>
-      <c r="AU1" s="86"/>
-      <c r="AV1" s="86"/>
-      <c r="AW1" s="86"/>
-      <c r="AX1" s="86"/>
-      <c r="AY1" s="86"/>
-      <c r="AZ1" s="86"/>
-      <c r="BA1" s="86"/>
-      <c r="BB1" s="86"/>
-      <c r="BC1" s="86"/>
-      <c r="BD1" s="86"/>
-      <c r="BE1" s="85" t="s">
+      <c r="AM1" s="110"/>
+      <c r="AN1" s="110"/>
+      <c r="AO1" s="110"/>
+      <c r="AP1" s="110"/>
+      <c r="AQ1" s="110"/>
+      <c r="AR1" s="110"/>
+      <c r="AS1" s="110"/>
+      <c r="AT1" s="110"/>
+      <c r="AU1" s="110"/>
+      <c r="AV1" s="110"/>
+      <c r="AW1" s="110"/>
+      <c r="AX1" s="110"/>
+      <c r="AY1" s="110"/>
+      <c r="AZ1" s="110"/>
+      <c r="BA1" s="110"/>
+      <c r="BB1" s="110"/>
+      <c r="BC1" s="110"/>
+      <c r="BD1" s="110"/>
+      <c r="BE1" s="109" t="s">
         <v>124</v>
       </c>
-      <c r="BF1" s="85"/>
-      <c r="BG1" s="85"/>
-      <c r="BH1" s="85"/>
-      <c r="BI1" s="82" t="s">
+      <c r="BF1" s="109"/>
+      <c r="BG1" s="109"/>
+      <c r="BH1" s="109"/>
+      <c r="BI1" s="107" t="s">
         <v>135</v>
       </c>
-      <c r="BJ1" s="82"/>
+      <c r="BJ1" s="107"/>
     </row>
     <row r="2" spans="1:62">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="84" t="s">
         <v>403</v>
       </c>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="105" t="s">
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="87" t="s">
         <v>398</v>
       </c>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
-      <c r="N2" s="105"/>
-      <c r="O2" s="105"/>
-      <c r="P2" s="105"/>
-      <c r="Q2" s="105"/>
-      <c r="R2" s="105"/>
-      <c r="S2" s="110" t="s">
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
+      <c r="N2" s="87"/>
+      <c r="O2" s="87"/>
+      <c r="P2" s="87"/>
+      <c r="Q2" s="87"/>
+      <c r="R2" s="87"/>
+      <c r="S2" s="94" t="s">
         <v>418</v>
       </c>
-      <c r="T2" s="110"/>
-      <c r="U2" s="110"/>
-      <c r="V2" s="111" t="s">
+      <c r="T2" s="94"/>
+      <c r="U2" s="94"/>
+      <c r="V2" s="95" t="s">
         <v>419</v>
       </c>
-      <c r="W2" s="111"/>
-      <c r="X2" s="111"/>
-      <c r="Y2" s="111"/>
-      <c r="Z2" s="112" t="s">
+      <c r="W2" s="95"/>
+      <c r="X2" s="95"/>
+      <c r="Y2" s="95"/>
+      <c r="Z2" s="96" t="s">
         <v>420</v>
       </c>
-      <c r="AA2" s="112"/>
-      <c r="AB2" s="112"/>
-      <c r="AC2" s="112"/>
-      <c r="AD2" s="112"/>
-      <c r="AE2" s="112"/>
-      <c r="AF2" s="112"/>
-      <c r="AG2" s="112"/>
-      <c r="AH2" s="112"/>
-      <c r="AI2" s="112"/>
-      <c r="AJ2" s="112"/>
-      <c r="AK2" s="112"/>
-      <c r="AL2" s="88" t="s">
+      <c r="AA2" s="96"/>
+      <c r="AB2" s="96"/>
+      <c r="AC2" s="96"/>
+      <c r="AD2" s="96"/>
+      <c r="AE2" s="96"/>
+      <c r="AF2" s="96"/>
+      <c r="AG2" s="96"/>
+      <c r="AH2" s="96"/>
+      <c r="AI2" s="96"/>
+      <c r="AJ2" s="96"/>
+      <c r="AK2" s="96"/>
+      <c r="AL2" s="112" t="s">
         <v>434</v>
       </c>
-      <c r="AM2" s="88"/>
-      <c r="AN2" s="88"/>
-      <c r="AO2" s="88"/>
-      <c r="AP2" s="88"/>
-      <c r="AQ2" s="88"/>
-      <c r="AR2" s="88"/>
-      <c r="AS2" s="89" t="s">
+      <c r="AM2" s="112"/>
+      <c r="AN2" s="112"/>
+      <c r="AO2" s="112"/>
+      <c r="AP2" s="112"/>
+      <c r="AQ2" s="112"/>
+      <c r="AR2" s="112"/>
+      <c r="AS2" s="113" t="s">
         <v>433</v>
       </c>
-      <c r="AT2" s="89"/>
-      <c r="AU2" s="89"/>
-      <c r="AV2" s="89"/>
-      <c r="AW2" s="89"/>
-      <c r="AX2" s="87" t="s">
+      <c r="AT2" s="113"/>
+      <c r="AU2" s="113"/>
+      <c r="AV2" s="113"/>
+      <c r="AW2" s="113"/>
+      <c r="AX2" s="111" t="s">
         <v>446</v>
       </c>
-      <c r="AY2" s="87"/>
-      <c r="AZ2" s="87"/>
-      <c r="BA2" s="87"/>
-      <c r="BB2" s="87"/>
-      <c r="BC2" s="84" t="s">
+      <c r="AY2" s="111"/>
+      <c r="AZ2" s="111"/>
+      <c r="BA2" s="111"/>
+      <c r="BB2" s="111"/>
+      <c r="BC2" s="99" t="s">
         <v>447</v>
       </c>
-      <c r="BD2" s="90" t="s">
+      <c r="BD2" s="86" t="s">
         <v>122</v>
       </c>
-      <c r="BE2" s="83" t="s">
+      <c r="BE2" s="108" t="s">
         <v>449</v>
       </c>
-      <c r="BF2" s="83" t="s">
+      <c r="BF2" s="108" t="s">
         <v>448</v>
       </c>
-      <c r="BG2" s="83" t="s">
+      <c r="BG2" s="108" t="s">
         <v>450</v>
       </c>
-      <c r="BH2" s="83" t="s">
+      <c r="BH2" s="108" t="s">
         <v>451</v>
       </c>
-      <c r="BI2" s="83" t="s">
+      <c r="BI2" s="108" t="s">
         <v>452</v>
       </c>
-      <c r="BJ2" s="83" t="s">
+      <c r="BJ2" s="108" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:62" ht="15" customHeight="1">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="86" t="s">
         <v>455</v>
       </c>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="103" t="s">
         <v>474</v>
       </c>
-      <c r="C3" s="106" t="s">
+      <c r="C3" s="88" t="s">
         <v>409</v>
       </c>
-      <c r="D3" s="80" t="s">
+      <c r="D3" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="80" t="s">
+      <c r="E3" s="90" t="s">
         <v>400</v>
       </c>
-      <c r="F3" s="80" t="s">
+      <c r="F3" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="81" t="s">
+      <c r="G3" s="91" t="s">
         <v>479</v>
       </c>
-      <c r="H3" s="80" t="s">
+      <c r="H3" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="108" t="s">
+      <c r="I3" s="92" t="s">
         <v>399</v>
       </c>
-      <c r="J3" s="108"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="108"/>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108"/>
-      <c r="O3" s="109" t="s">
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="92"/>
+      <c r="O3" s="93" t="s">
         <v>405</v>
       </c>
-      <c r="P3" s="109"/>
-      <c r="Q3" s="109"/>
-      <c r="R3" s="109"/>
-      <c r="S3" s="80" t="s">
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="93"/>
+      <c r="S3" s="90" t="s">
         <v>416</v>
       </c>
-      <c r="T3" s="80" t="s">
+      <c r="T3" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="U3" s="98" t="s">
+      <c r="U3" s="97" t="s">
         <v>477</v>
       </c>
-      <c r="V3" s="98" t="s">
+      <c r="V3" s="97" t="s">
         <v>55</v>
       </c>
-      <c r="W3" s="80" t="s">
+      <c r="W3" s="90" t="s">
         <v>421</v>
       </c>
-      <c r="X3" s="99" t="s">
+      <c r="X3" s="98" t="s">
         <v>424</v>
       </c>
-      <c r="Y3" s="81" t="s">
+      <c r="Y3" s="91" t="s">
         <v>478</v>
       </c>
-      <c r="Z3" s="80" t="s">
+      <c r="Z3" s="90" t="s">
         <v>426</v>
       </c>
-      <c r="AA3" s="81" t="s">
+      <c r="AA3" s="91" t="s">
         <v>69</v>
       </c>
-      <c r="AB3" s="80" t="s">
+      <c r="AB3" s="90" t="s">
         <v>427</v>
       </c>
-      <c r="AC3" s="80" t="s">
+      <c r="AC3" s="90" t="s">
         <v>429</v>
       </c>
-      <c r="AD3" s="81" t="s">
+      <c r="AD3" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="AE3" s="81" t="s">
+      <c r="AE3" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="AF3" s="81" t="s">
+      <c r="AF3" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="AG3" s="80" t="s">
+      <c r="AG3" s="90" t="s">
         <v>428</v>
       </c>
-      <c r="AH3" s="80" t="s">
+      <c r="AH3" s="90" t="s">
         <v>430</v>
       </c>
-      <c r="AI3" s="81" t="s">
+      <c r="AI3" s="91" t="s">
         <v>85</v>
       </c>
-      <c r="AJ3" s="93" t="s">
+      <c r="AJ3" s="105" t="s">
         <v>468</v>
       </c>
-      <c r="AK3" s="80" t="s">
+      <c r="AK3" s="90" t="s">
         <v>431</v>
       </c>
-      <c r="AL3" s="97" t="s">
+      <c r="AL3" s="100" t="s">
         <v>435</v>
       </c>
-      <c r="AM3" s="97" t="s">
+      <c r="AM3" s="100" t="s">
         <v>437</v>
       </c>
-      <c r="AN3" s="97" t="s">
+      <c r="AN3" s="100" t="s">
         <v>438</v>
       </c>
-      <c r="AO3" s="95" t="s">
+      <c r="AO3" s="101" t="s">
         <v>464</v>
       </c>
-      <c r="AP3" s="97" t="s">
+      <c r="AP3" s="100" t="s">
         <v>439</v>
       </c>
-      <c r="AQ3" s="95" t="s">
+      <c r="AQ3" s="101" t="s">
         <v>465</v>
       </c>
-      <c r="AR3" s="97" t="s">
+      <c r="AR3" s="100" t="s">
         <v>440</v>
       </c>
-      <c r="AS3" s="90" t="s">
+      <c r="AS3" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="AT3" s="84" t="s">
+      <c r="AT3" s="99" t="s">
         <v>441</v>
       </c>
-      <c r="AU3" s="84" t="s">
+      <c r="AU3" s="99" t="s">
         <v>442</v>
       </c>
-      <c r="AV3" s="84" t="s">
+      <c r="AV3" s="99" t="s">
         <v>443</v>
       </c>
-      <c r="AW3" s="84" t="s">
+      <c r="AW3" s="99" t="s">
         <v>445</v>
       </c>
-      <c r="AX3" s="84" t="s">
+      <c r="AX3" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="AY3" s="84" t="s">
+      <c r="AY3" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="AZ3" s="84" t="s">
+      <c r="AZ3" s="99" t="s">
         <v>114</v>
       </c>
-      <c r="BA3" s="84" t="s">
+      <c r="BA3" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="BB3" s="84" t="s">
+      <c r="BB3" s="99" t="s">
         <v>118</v>
       </c>
-      <c r="BC3" s="84"/>
-      <c r="BD3" s="90"/>
-      <c r="BE3" s="83"/>
-      <c r="BF3" s="83"/>
-      <c r="BG3" s="83"/>
-      <c r="BH3" s="83"/>
-      <c r="BI3" s="83"/>
-      <c r="BJ3" s="83"/>
+      <c r="BC3" s="99"/>
+      <c r="BD3" s="86"/>
+      <c r="BE3" s="108"/>
+      <c r="BF3" s="108"/>
+      <c r="BG3" s="108"/>
+      <c r="BH3" s="108"/>
+      <c r="BI3" s="108"/>
+      <c r="BJ3" s="108"/>
     </row>
     <row r="4" spans="1:62">
-      <c r="A4" s="90"/>
-      <c r="B4" s="92"/>
-      <c r="C4" s="107"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
+      <c r="A4" s="86"/>
+      <c r="B4" s="104"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
       <c r="I4" s="20" t="s">
         <v>401</v>
       </c>
@@ -8785,50 +8798,50 @@
       <c r="R4" s="20" t="s">
         <v>415</v>
       </c>
-      <c r="S4" s="80"/>
-      <c r="T4" s="80"/>
-      <c r="U4" s="98"/>
-      <c r="V4" s="98"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="98"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="80"/>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="80"/>
-      <c r="AC4" s="80"/>
-      <c r="AD4" s="81"/>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="81"/>
-      <c r="AG4" s="80"/>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="94"/>
-      <c r="AK4" s="80"/>
-      <c r="AL4" s="97"/>
-      <c r="AM4" s="97"/>
-      <c r="AN4" s="97"/>
-      <c r="AO4" s="96"/>
-      <c r="AP4" s="97"/>
-      <c r="AQ4" s="96"/>
-      <c r="AR4" s="97"/>
-      <c r="AS4" s="90"/>
-      <c r="AT4" s="84"/>
-      <c r="AU4" s="84"/>
-      <c r="AV4" s="84"/>
-      <c r="AW4" s="84"/>
-      <c r="AX4" s="84"/>
-      <c r="AY4" s="84"/>
-      <c r="AZ4" s="84"/>
-      <c r="BA4" s="84"/>
-      <c r="BB4" s="84"/>
-      <c r="BC4" s="84"/>
-      <c r="BD4" s="90"/>
-      <c r="BE4" s="83"/>
-      <c r="BF4" s="83"/>
-      <c r="BG4" s="83"/>
-      <c r="BH4" s="83"/>
-      <c r="BI4" s="83"/>
-      <c r="BJ4" s="83"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="97"/>
+      <c r="V4" s="97"/>
+      <c r="W4" s="91"/>
+      <c r="X4" s="97"/>
+      <c r="Y4" s="90"/>
+      <c r="Z4" s="90"/>
+      <c r="AA4" s="91"/>
+      <c r="AB4" s="90"/>
+      <c r="AC4" s="90"/>
+      <c r="AD4" s="91"/>
+      <c r="AE4" s="91"/>
+      <c r="AF4" s="91"/>
+      <c r="AG4" s="90"/>
+      <c r="AH4" s="91"/>
+      <c r="AI4" s="91"/>
+      <c r="AJ4" s="106"/>
+      <c r="AK4" s="90"/>
+      <c r="AL4" s="100"/>
+      <c r="AM4" s="100"/>
+      <c r="AN4" s="100"/>
+      <c r="AO4" s="102"/>
+      <c r="AP4" s="100"/>
+      <c r="AQ4" s="102"/>
+      <c r="AR4" s="100"/>
+      <c r="AS4" s="86"/>
+      <c r="AT4" s="99"/>
+      <c r="AU4" s="99"/>
+      <c r="AV4" s="99"/>
+      <c r="AW4" s="99"/>
+      <c r="AX4" s="99"/>
+      <c r="AY4" s="99"/>
+      <c r="AZ4" s="99"/>
+      <c r="BA4" s="99"/>
+      <c r="BB4" s="99"/>
+      <c r="BC4" s="99"/>
+      <c r="BD4" s="86"/>
+      <c r="BE4" s="108"/>
+      <c r="BF4" s="108"/>
+      <c r="BG4" s="108"/>
+      <c r="BH4" s="108"/>
+      <c r="BI4" s="108"/>
+      <c r="BJ4" s="108"/>
     </row>
     <row r="5" spans="1:62">
       <c r="A5" s="21"/>
@@ -9478,67 +9491,100 @@
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:47">
       <c r="A17" s="26"/>
       <c r="B17" s="26"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:47">
       <c r="A18" s="26"/>
       <c r="B18" s="26"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:47">
       <c r="A19" s="26"/>
       <c r="B19" s="26"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:47">
       <c r="A20" s="26"/>
       <c r="B20" s="26"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:47">
       <c r="A21" s="26"/>
       <c r="B21" s="26"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:47">
       <c r="A22" s="26"/>
       <c r="B22" s="26"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:47">
       <c r="A23" s="26"/>
       <c r="B23" s="26"/>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="AK23" t="s">
+        <v>435</v>
+      </c>
+      <c r="AL23" t="s">
+        <v>437</v>
+      </c>
+      <c r="AM23" t="s">
+        <v>438</v>
+      </c>
+      <c r="AN23" t="s">
+        <v>464</v>
+      </c>
+      <c r="AO23" t="s">
+        <v>439</v>
+      </c>
+      <c r="AP23" t="s">
+        <v>465</v>
+      </c>
+      <c r="AQ23" t="s">
+        <v>440</v>
+      </c>
+      <c r="AR23" t="s">
+        <v>99</v>
+      </c>
+      <c r="AS23" t="s">
+        <v>441</v>
+      </c>
+      <c r="AT23" t="s">
+        <v>442</v>
+      </c>
+      <c r="AU23" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="24" spans="1:47">
       <c r="A24" s="26"/>
       <c r="B24" s="26"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:47">
       <c r="A25" s="26"/>
       <c r="B25" s="26"/>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:47">
       <c r="A26" s="26"/>
       <c r="B26" s="26"/>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:47">
       <c r="A27" s="26"/>
       <c r="B27" s="26"/>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:47">
       <c r="A28" s="26"/>
       <c r="B28" s="26"/>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:47">
       <c r="A29" s="26"/>
       <c r="B29" s="26"/>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:47">
       <c r="A30" s="26"/>
       <c r="B30" s="26"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:47">
       <c r="A31" s="26"/>
       <c r="B31" s="26"/>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:47">
       <c r="A32" s="26"/>
       <c r="B32" s="26"/>
     </row>
@@ -10325,6 +10371,57 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="67">
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="BI1:BJ1"/>
+    <mergeCell ref="BI2:BI4"/>
+    <mergeCell ref="BJ2:BJ4"/>
+    <mergeCell ref="BA3:BA4"/>
+    <mergeCell ref="BB3:BB4"/>
+    <mergeCell ref="BE1:BH1"/>
+    <mergeCell ref="BE2:BE4"/>
+    <mergeCell ref="BF2:BF4"/>
+    <mergeCell ref="BG2:BG4"/>
+    <mergeCell ref="BH2:BH4"/>
+    <mergeCell ref="AL1:BD1"/>
+    <mergeCell ref="AX2:BB2"/>
+    <mergeCell ref="AL2:AR2"/>
+    <mergeCell ref="AS2:AW2"/>
+    <mergeCell ref="BD2:BD4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AJ3:AJ4"/>
+    <mergeCell ref="AT3:AT4"/>
+    <mergeCell ref="AU3:AU4"/>
+    <mergeCell ref="AQ3:AQ4"/>
+    <mergeCell ref="AG3:AG4"/>
+    <mergeCell ref="AH3:AH4"/>
+    <mergeCell ref="AI3:AI4"/>
+    <mergeCell ref="AK3:AK4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="BC2:BC4"/>
+    <mergeCell ref="AL3:AL4"/>
+    <mergeCell ref="AM3:AM4"/>
+    <mergeCell ref="AN3:AN4"/>
+    <mergeCell ref="AP3:AP4"/>
+    <mergeCell ref="AR3:AR4"/>
+    <mergeCell ref="AS3:AS4"/>
+    <mergeCell ref="AW3:AW4"/>
+    <mergeCell ref="AX3:AX4"/>
+    <mergeCell ref="AY3:AY4"/>
+    <mergeCell ref="AZ3:AZ4"/>
+    <mergeCell ref="AO3:AO4"/>
+    <mergeCell ref="AV3:AV4"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
     <mergeCell ref="S1:AK1"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A2:F2"/>
@@ -10341,57 +10438,6 @@
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="Z2:AK2"/>
     <mergeCell ref="S3:S4"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="BC2:BC4"/>
-    <mergeCell ref="AL3:AL4"/>
-    <mergeCell ref="AM3:AM4"/>
-    <mergeCell ref="AN3:AN4"/>
-    <mergeCell ref="AP3:AP4"/>
-    <mergeCell ref="AR3:AR4"/>
-    <mergeCell ref="AS3:AS4"/>
-    <mergeCell ref="AW3:AW4"/>
-    <mergeCell ref="AX3:AX4"/>
-    <mergeCell ref="AY3:AY4"/>
-    <mergeCell ref="AZ3:AZ4"/>
-    <mergeCell ref="AO3:AO4"/>
-    <mergeCell ref="AV3:AV4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AJ3:AJ4"/>
-    <mergeCell ref="AT3:AT4"/>
-    <mergeCell ref="AU3:AU4"/>
-    <mergeCell ref="AQ3:AQ4"/>
-    <mergeCell ref="AG3:AG4"/>
-    <mergeCell ref="AH3:AH4"/>
-    <mergeCell ref="AI3:AI4"/>
-    <mergeCell ref="AK3:AK4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="BI1:BJ1"/>
-    <mergeCell ref="BI2:BI4"/>
-    <mergeCell ref="BJ2:BJ4"/>
-    <mergeCell ref="BA3:BA4"/>
-    <mergeCell ref="BB3:BB4"/>
-    <mergeCell ref="BE1:BH1"/>
-    <mergeCell ref="BE2:BE4"/>
-    <mergeCell ref="BF2:BF4"/>
-    <mergeCell ref="BG2:BG4"/>
-    <mergeCell ref="BH2:BH4"/>
-    <mergeCell ref="AL1:BD1"/>
-    <mergeCell ref="AX2:BB2"/>
-    <mergeCell ref="AL2:AR2"/>
-    <mergeCell ref="AS2:AW2"/>
-    <mergeCell ref="BD2:BD4"/>
   </mergeCells>
   <dataValidations xWindow="597" yWindow="252" count="91">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Gametocytes present" sqref="AS3"/>
@@ -12063,7 +12109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
@@ -12095,12 +12141,12 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="115"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="116"/>
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5">
@@ -12315,12 +12361,12 @@
       <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="116" t="s">
+      <c r="A18" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="117"/>
-      <c r="C18" s="117"/>
-      <c r="D18" s="118"/>
+      <c r="B18" s="118"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="119"/>
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" ht="28">
@@ -12605,12 +12651,12 @@
       <c r="E37" s="13"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="119" t="s">
+      <c r="A38" s="120" t="s">
         <v>89</v>
       </c>
-      <c r="B38" s="120"/>
-      <c r="C38" s="120"/>
-      <c r="D38" s="121"/>
+      <c r="B38" s="121"/>
+      <c r="C38" s="121"/>
+      <c r="D38" s="122"/>
       <c r="E38" s="13"/>
     </row>
     <row r="39" spans="1:5" ht="42">
@@ -12881,13 +12927,13 @@
       <c r="E57" s="13"/>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="122" t="s">
+      <c r="A58" s="123" t="s">
         <v>124</v>
       </c>
-      <c r="B58" s="123"/>
-      <c r="C58" s="123"/>
-      <c r="D58" s="123"/>
-      <c r="E58" s="123"/>
+      <c r="B58" s="124"/>
+      <c r="C58" s="124"/>
+      <c r="D58" s="124"/>
+      <c r="E58" s="124"/>
     </row>
     <row r="59" spans="1:5" ht="28">
       <c r="A59" s="15" t="s">
@@ -12950,12 +12996,12 @@
       <c r="E62" s="15"/>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="124" t="s">
+      <c r="A63" s="125" t="s">
         <v>135</v>
       </c>
-      <c r="B63" s="124"/>
-      <c r="C63" s="124"/>
-      <c r="D63" s="125"/>
+      <c r="B63" s="125"/>
+      <c r="C63" s="125"/>
+      <c r="D63" s="126"/>
       <c r="E63" s="15"/>
     </row>
     <row r="64" spans="1:5" ht="70">

</xml_diff>